<commit_message>
literacy, 240930 modified 2
</commit_message>
<xml_diff>
--- a/R/data/literacy_240930.xlsx
+++ b/R/data/literacy_240930.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7723BCEF-3833-0A47-9F89-3D782D38845F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BACCAC6-3519-C24E-890B-D2D068674156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50400" yWindow="1360" windowWidth="44800" windowHeight="24700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3000" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3648" uniqueCount="450">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -1205,6 +1205,171 @@
   </si>
   <si>
     <t>동형원</t>
+  </si>
+  <si>
+    <t>jungha051026@naver.com</t>
+  </si>
+  <si>
+    <t>윤정하</t>
+  </si>
+  <si>
+    <t>junsa215909@naver.com</t>
+  </si>
+  <si>
+    <t>이승준</t>
+  </si>
+  <si>
+    <t>chlrkdus5@naver.com</t>
+  </si>
+  <si>
+    <t>최가연</t>
+  </si>
+  <si>
+    <t>csyoon1215@naver.com</t>
+  </si>
+  <si>
+    <t>천세윤</t>
+  </si>
+  <si>
+    <t>ye_ji_02@naver.com</t>
+  </si>
+  <si>
+    <t>전예지</t>
+  </si>
+  <si>
+    <t>dkaldmswl05@gmail.com</t>
+  </si>
+  <si>
+    <t>엄은지</t>
+  </si>
+  <si>
+    <t>zmgofk1591@gmail.com</t>
+  </si>
+  <si>
+    <t>AI로봇융합</t>
+  </si>
+  <si>
+    <t>박하늘</t>
+  </si>
+  <si>
+    <t>jh2600646@naver.com</t>
+  </si>
+  <si>
+    <t>데이터사이언스</t>
+  </si>
+  <si>
+    <t>박지훈</t>
+  </si>
+  <si>
+    <t>ejsl5231@gmail.com</t>
+  </si>
+  <si>
+    <t>디지털미디어콘텐츠학과</t>
+  </si>
+  <si>
+    <t>이유찬</t>
+  </si>
+  <si>
+    <t>ji040414@naver.com</t>
+  </si>
+  <si>
+    <t>최윤지</t>
+  </si>
+  <si>
+    <t>herdy2154@naver.com</t>
+  </si>
+  <si>
+    <t>한녕균</t>
+  </si>
+  <si>
+    <t>oepdwrtyy@gmail.com</t>
+  </si>
+  <si>
+    <t>강종현</t>
+  </si>
+  <si>
+    <t>sin50407899@gmail.com</t>
+  </si>
+  <si>
+    <t>신재화</t>
+  </si>
+  <si>
+    <t>bin_1014@naver.com</t>
+  </si>
+  <si>
+    <t>디지털미디어콘텐츠 전공</t>
+  </si>
+  <si>
+    <t>김명빈</t>
+  </si>
+  <si>
+    <t>detect5641@gmail.com</t>
+  </si>
+  <si>
+    <t>이주성</t>
+  </si>
+  <si>
+    <t>dpdlvldzmfkd1218@naver.com</t>
+  </si>
+  <si>
+    <t>이다혜</t>
+  </si>
+  <si>
+    <t>minseok1937@gmail.com</t>
+  </si>
+  <si>
+    <t>김민석</t>
+  </si>
+  <si>
+    <t>lucy1004486@naver.com</t>
+  </si>
+  <si>
+    <t>김소연</t>
+  </si>
+  <si>
+    <t>kkst1324@naver.com</t>
+  </si>
+  <si>
+    <t>국어국문학과</t>
+  </si>
+  <si>
+    <t>구민영</t>
+  </si>
+  <si>
+    <t>kang__bbo@naver.com</t>
+  </si>
+  <si>
+    <t>미래융합스쿨</t>
+  </si>
+  <si>
+    <t>강다은</t>
+  </si>
+  <si>
+    <t>gyucheol0503@naver.com</t>
+  </si>
+  <si>
+    <t>홍규철</t>
+  </si>
+  <si>
+    <t>pcw5766@naver.com</t>
+  </si>
+  <si>
+    <t>광고홍보학과</t>
+  </si>
+  <si>
+    <t>박찬웅</t>
+  </si>
+  <si>
+    <t>woosm050530@gmail.com</t>
+  </si>
+  <si>
+    <t>우수민</t>
+  </si>
+  <si>
+    <t>b020305@naver.com</t>
+  </si>
+  <si>
+    <t>배성진</t>
   </si>
 </sst>
 </file>
@@ -1571,7 +1736,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:AD111">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:AD135">
   <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -1809,11 +1974,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD111"/>
+  <dimension ref="A1:AD135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E120" sqref="E120"/>
+      <selection pane="bottomLeft" activeCell="D139" sqref="D139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -12058,6 +12223,2214 @@
         <v>56</v>
       </c>
     </row>
+    <row r="112" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A112" s="4">
+        <v>45566.832590497681</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D112" s="5">
+        <v>20245213</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="F112" s="5">
+        <v>3</v>
+      </c>
+      <c r="G112" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H112" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I112" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="J112" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="K112" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="L112" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="M112" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N112" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O112" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="P112" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q112" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="R112" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="S112" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T112" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U112" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="V112" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="W112" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="X112" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="Y112" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z112" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA112" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB112" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="AC112" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD112" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="113" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A113" s="7">
+        <v>45566.842430578705</v>
+      </c>
+      <c r="B113" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="C113" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D113" s="8">
+        <v>20203006</v>
+      </c>
+      <c r="E113" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="F113" s="8">
+        <v>3</v>
+      </c>
+      <c r="G113" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="H113" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I113" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J113" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="K113" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L113" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M113" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N113" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O113" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="P113" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q113" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R113" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="S113" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T113" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U113" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V113" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W113" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X113" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y113" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z113" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA113" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB113" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC113" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD113" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="114" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A114" s="4">
+        <v>45566.843356377314</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D114" s="5">
+        <v>20246294</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="F114" s="5">
+        <v>3</v>
+      </c>
+      <c r="G114" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H114" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I114" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J114" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K114" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L114" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M114" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="N114" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O114" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P114" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q114" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R114" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S114" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="T114" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U114" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V114" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W114" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X114" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y114" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z114" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA114" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB114" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC114" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD114" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="115" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A115" s="7">
+        <v>45566.851832187502</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="C115" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D115" s="8">
+        <v>20246292</v>
+      </c>
+      <c r="E115" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="F115" s="8">
+        <v>3</v>
+      </c>
+      <c r="G115" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H115" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I115" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J115" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K115" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L115" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M115" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N115" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O115" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P115" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q115" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R115" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S115" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T115" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U115" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V115" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W115" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X115" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y115" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z115" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA115" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB115" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC115" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD115" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="116" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A116" s="4">
+        <v>45566.859180520834</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D116" s="5">
+        <v>20213839</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="F116" s="5">
+        <v>3</v>
+      </c>
+      <c r="G116" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H116" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I116" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J116" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K116" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L116" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M116" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N116" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O116" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P116" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q116" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R116" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S116" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T116" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U116" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V116" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W116" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X116" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y116" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z116" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA116" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB116" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC116" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD116" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="117" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A117" s="7">
+        <v>45566.863790138887</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="C117" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D117" s="8">
+        <v>20221059</v>
+      </c>
+      <c r="E117" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="F117" s="8">
+        <v>3</v>
+      </c>
+      <c r="G117" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H117" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I117" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J117" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K117" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L117" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M117" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N117" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O117" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P117" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q117" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R117" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S117" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T117" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="U117" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="V117" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="W117" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X117" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y117" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z117" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA117" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB117" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC117" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD117" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="118" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A118" s="4">
+        <v>45566.872440381943</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="D118" s="5">
+        <v>20216731</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="F118" s="5">
+        <v>3</v>
+      </c>
+      <c r="G118" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H118" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I118" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J118" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K118" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L118" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M118" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N118" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O118" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P118" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q118" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R118" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S118" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T118" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U118" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V118" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W118" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X118" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y118" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z118" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA118" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB118" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC118" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD118" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="119" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A119" s="7">
+        <v>45566.875019340281</v>
+      </c>
+      <c r="B119" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="C119" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="D119" s="8">
+        <v>20213224</v>
+      </c>
+      <c r="E119" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="F119" s="8">
+        <v>3</v>
+      </c>
+      <c r="G119" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H119" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I119" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J119" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K119" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L119" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M119" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N119" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O119" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P119" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q119" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R119" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S119" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T119" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U119" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V119" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W119" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X119" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y119" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z119" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA119" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB119" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC119" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD119" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="120" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A120" s="4">
+        <v>45566.880075335648</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="D120" s="5">
+        <v>20225223</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="F120" s="5">
+        <v>3</v>
+      </c>
+      <c r="G120" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H120" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I120" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J120" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K120" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L120" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M120" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N120" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O120" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P120" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q120" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R120" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S120" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T120" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U120" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V120" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W120" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X120" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y120" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z120" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA120" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB120" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC120" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD120" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="121" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A121" s="7">
+        <v>45566.892236006941</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="C121" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D121" s="8">
+        <v>20233055</v>
+      </c>
+      <c r="E121" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="F121" s="8">
+        <v>3</v>
+      </c>
+      <c r="G121" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H121" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I121" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J121" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="K121" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L121" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M121" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N121" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O121" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P121" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q121" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R121" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S121" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T121" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U121" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V121" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W121" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X121" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y121" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z121" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA121" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB121" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC121" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD121" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="122" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A122" s="4">
+        <v>45566.892452442131</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="C122" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D122" s="5">
+        <v>20193010</v>
+      </c>
+      <c r="E122" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="F122" s="5">
+        <v>3</v>
+      </c>
+      <c r="G122" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H122" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I122" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J122" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K122" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="L122" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M122" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N122" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O122" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P122" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q122" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R122" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S122" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T122" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U122" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V122" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W122" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X122" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y122" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z122" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA122" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB122" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC122" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD122" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="123" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A123" s="7">
+        <v>45566.901903819446</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="C123" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D123" s="8">
+        <v>20241003</v>
+      </c>
+      <c r="E123" s="8" t="s">
+        <v>421</v>
+      </c>
+      <c r="F123" s="8">
+        <v>3</v>
+      </c>
+      <c r="G123" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H123" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I123" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J123" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K123" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L123" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M123" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N123" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O123" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P123" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q123" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R123" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S123" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T123" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U123" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V123" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W123" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X123" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y123" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z123" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA123" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB123" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC123" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD123" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="124" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A124" s="4">
+        <v>45566.943431331019</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D124" s="5">
+        <v>20202538</v>
+      </c>
+      <c r="E124" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="F124" s="5">
+        <v>3</v>
+      </c>
+      <c r="G124" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H124" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I124" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J124" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K124" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L124" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M124" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N124" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O124" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P124" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q124" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R124" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S124" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T124" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U124" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V124" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W124" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X124" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y124" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z124" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA124" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB124" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC124" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD124" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="125" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A125" s="7">
+        <v>45566.955206990737</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="C125" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="D125" s="8">
+        <v>20202706</v>
+      </c>
+      <c r="E125" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="F125" s="8">
+        <v>3</v>
+      </c>
+      <c r="G125" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H125" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I125" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J125" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K125" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L125" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M125" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N125" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O125" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P125" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q125" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R125" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S125" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T125" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U125" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V125" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W125" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X125" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y125" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z125" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA125" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB125" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC125" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD125" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="126" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A126" s="4">
+        <v>45566.972859745365</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="C126" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D126" s="5">
+        <v>20245230</v>
+      </c>
+      <c r="E126" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="F126" s="5">
+        <v>3</v>
+      </c>
+      <c r="G126" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H126" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I126" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J126" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K126" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="L126" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M126" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N126" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O126" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P126" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q126" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R126" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S126" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="T126" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="U126" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="V126" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W126" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X126" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y126" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z126" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA126" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB126" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC126" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD126" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="127" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A127" s="7">
+        <v>45566.975056597221</v>
+      </c>
+      <c r="B127" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="C127" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D127" s="8">
+        <v>20243933</v>
+      </c>
+      <c r="E127" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="F127" s="8">
+        <v>3</v>
+      </c>
+      <c r="G127" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H127" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I127" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J127" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K127" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L127" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M127" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N127" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O127" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P127" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q127" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R127" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S127" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T127" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U127" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V127" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W127" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X127" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y127" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z127" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA127" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB127" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC127" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD127" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="128" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A128" s="4">
+        <v>45566.986494050929</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="C128" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D128" s="5">
+        <v>20202915</v>
+      </c>
+      <c r="E128" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="F128" s="5">
+        <v>3</v>
+      </c>
+      <c r="G128" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H128" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I128" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J128" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K128" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L128" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M128" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N128" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O128" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P128" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q128" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R128" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S128" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T128" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U128" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V128" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W128" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X128" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y128" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z128" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA128" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB128" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC128" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD128" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="129" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A129" s="7">
+        <v>45566.989290590282</v>
+      </c>
+      <c r="B129" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="C129" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D129" s="8">
+        <v>20232512</v>
+      </c>
+      <c r="E129" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="F129" s="8">
+        <v>3</v>
+      </c>
+      <c r="G129" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H129" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I129" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J129" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K129" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L129" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M129" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N129" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O129" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P129" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q129" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R129" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S129" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T129" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U129" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V129" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W129" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X129" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y129" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z129" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA129" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB129" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC129" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD129" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="130" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A130" s="4">
+        <v>45566.992675023153</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="C130" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="D130" s="5">
+        <v>20201004</v>
+      </c>
+      <c r="E130" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="F130" s="5">
+        <v>3</v>
+      </c>
+      <c r="G130" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H130" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I130" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J130" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K130" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L130" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M130" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N130" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O130" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P130" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q130" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R130" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S130" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T130" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U130" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V130" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W130" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X130" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y130" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z130" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA130" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB130" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC130" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD130" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="131" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A131" s="7">
+        <v>45567.006227013888</v>
+      </c>
+      <c r="B131" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="C131" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="D131" s="8">
+        <v>20246601</v>
+      </c>
+      <c r="E131" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="F131" s="8">
+        <v>3</v>
+      </c>
+      <c r="G131" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H131" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I131" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J131" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="K131" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="L131" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M131" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="N131" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O131" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P131" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q131" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R131" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S131" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T131" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="U131" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="V131" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W131" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X131" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y131" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z131" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA131" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB131" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC131" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="AD131" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="132" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A132" s="4">
+        <v>45567.013628032408</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D132" s="5">
+        <v>20236650</v>
+      </c>
+      <c r="E132" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="F132" s="5">
+        <v>3</v>
+      </c>
+      <c r="G132" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="H132" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I132" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J132" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="K132" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L132" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M132" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N132" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O132" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P132" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q132" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R132" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S132" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T132" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="U132" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V132" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W132" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X132" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y132" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z132" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA132" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB132" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC132" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD132" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="133" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A133" s="7">
+        <v>45567.024706759257</v>
+      </c>
+      <c r="B133" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="C133" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="D133" s="8">
+        <v>20192616</v>
+      </c>
+      <c r="E133" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="F133" s="8">
+        <v>1</v>
+      </c>
+      <c r="G133" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="H133" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I133" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="J133" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K133" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L133" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M133" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="N133" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O133" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="P133" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q133" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="R133" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="S133" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="T133" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="U133" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="V133" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="W133" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="X133" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y133" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z133" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="AA133" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB133" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC133" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD133" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="134" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A134" s="4">
+        <v>45567.028664050929</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D134" s="5">
+        <v>20243630</v>
+      </c>
+      <c r="E134" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="F134" s="5">
+        <v>3</v>
+      </c>
+      <c r="G134" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H134" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I134" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J134" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K134" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L134" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M134" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N134" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O134" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P134" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q134" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R134" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S134" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T134" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="U134" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V134" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W134" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X134" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y134" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z134" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA134" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB134" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC134" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD134" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="135" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A135" s="13">
+        <v>45567.06748946759</v>
+      </c>
+      <c r="B135" s="14" t="s">
+        <v>448</v>
+      </c>
+      <c r="C135" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="D135" s="14">
+        <v>20212418</v>
+      </c>
+      <c r="E135" s="14" t="s">
+        <v>449</v>
+      </c>
+      <c r="F135" s="14">
+        <v>3</v>
+      </c>
+      <c r="G135" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H135" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="I135" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J135" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="K135" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="L135" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="M135" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N135" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="O135" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P135" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q135" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="R135" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="S135" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="T135" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="U135" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="V135" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="W135" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="X135" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y135" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z135" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA135" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB135" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC135" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD135" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
literacy, 240930 modified 4
</commit_message>
<xml_diff>
--- a/R/data/literacy_240930.xlsx
+++ b/R/data/literacy_240930.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE045A40-FA14-134A-AD74-FEC8907C7394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6AB34EE-90B2-E747-89E4-5665D308EC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50400" yWindow="1360" windowWidth="44800" windowHeight="24700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5079" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5592" uniqueCount="601">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -1706,6 +1706,123 @@
   </si>
   <si>
     <t xml:space="preserve">박기택 </t>
+  </si>
+  <si>
+    <t>raon02271@naver.com</t>
+  </si>
+  <si>
+    <t>이채윤</t>
+  </si>
+  <si>
+    <t>ye1651@naver.com</t>
+  </si>
+  <si>
+    <t>전예은</t>
+  </si>
+  <si>
+    <t>leeeunbi0717@naver.com</t>
+  </si>
+  <si>
+    <t>이은비</t>
+  </si>
+  <si>
+    <t>wogh1587@naver.com</t>
+  </si>
+  <si>
+    <t>현재호</t>
+  </si>
+  <si>
+    <t>wlduddember6@gmail.com</t>
+  </si>
+  <si>
+    <t>이지영</t>
+  </si>
+  <si>
+    <t>gomdolri05@naver.com</t>
+  </si>
+  <si>
+    <t>이아영</t>
+  </si>
+  <si>
+    <t>ming041230@gmail.com</t>
+  </si>
+  <si>
+    <t>joo061222@gmail.com</t>
+  </si>
+  <si>
+    <t>강민주</t>
+  </si>
+  <si>
+    <t>baeseung1211@gmail.com</t>
+  </si>
+  <si>
+    <t>배승혁</t>
+  </si>
+  <si>
+    <t>jenniferdy@naver.com</t>
+  </si>
+  <si>
+    <t>권도연</t>
+  </si>
+  <si>
+    <t>0214lily@naver.com</t>
+  </si>
+  <si>
+    <t>김가희</t>
+  </si>
+  <si>
+    <t>jaehun081805@gmail.com</t>
+  </si>
+  <si>
+    <t>이재훈</t>
+  </si>
+  <si>
+    <t>cindy_lol@naver.com</t>
+  </si>
+  <si>
+    <t>국어국문학전공</t>
+  </si>
+  <si>
+    <t>권한별</t>
+  </si>
+  <si>
+    <t>narinsong3@gmail.com</t>
+  </si>
+  <si>
+    <t>송나린</t>
+  </si>
+  <si>
+    <t>hijgc8282@naver.com</t>
+  </si>
+  <si>
+    <t>윤장근</t>
+  </si>
+  <si>
+    <t>rlaskrud0917@naver.com</t>
+  </si>
+  <si>
+    <t>김나경</t>
+  </si>
+  <si>
+    <t>aldidrhemdgkrry1234@naver.com</t>
+  </si>
+  <si>
+    <t>영어영문</t>
+  </si>
+  <si>
+    <t>김용우</t>
+  </si>
+  <si>
+    <t>rhkwp0323@gmail.com</t>
+  </si>
+  <si>
+    <t>유도영</t>
+  </si>
+  <si>
+    <t>qaz5316qaz@naver.com</t>
+  </si>
+  <si>
+    <t>이동기</t>
   </si>
 </sst>
 </file>
@@ -2120,7 +2237,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:AD188">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:AD207">
   <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -2358,11 +2475,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD188"/>
+  <dimension ref="A1:AD207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C196" sqref="C196"/>
+      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D221" sqref="D221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -19691,6 +19808,1754 @@
         <v>132</v>
       </c>
     </row>
+    <row r="189" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A189" s="7">
+        <v>45568.517370706017</v>
+      </c>
+      <c r="B189" s="8" t="s">
+        <v>562</v>
+      </c>
+      <c r="C189" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D189" s="8">
+        <v>20233954</v>
+      </c>
+      <c r="E189" s="8" t="s">
+        <v>563</v>
+      </c>
+      <c r="F189" s="8">
+        <v>3</v>
+      </c>
+      <c r="G189" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H189" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I189" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J189" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K189" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L189" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M189" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N189" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O189" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P189" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q189" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R189" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S189" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T189" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U189" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V189" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W189" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X189" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y189" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z189" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA189" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB189" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC189" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD189" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="190" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A190" s="4">
+        <v>45568.533820173616</v>
+      </c>
+      <c r="B190" s="5" t="s">
+        <v>564</v>
+      </c>
+      <c r="C190" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D190" s="5">
+        <v>20243949</v>
+      </c>
+      <c r="E190" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="F190" s="5">
+        <v>3</v>
+      </c>
+      <c r="G190" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H190" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I190" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J190" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K190" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L190" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M190" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N190" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O190" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P190" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q190" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R190" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S190" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T190" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U190" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V190" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W190" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X190" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y190" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z190" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA190" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB190" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC190" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD190" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="191" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A191" s="7">
+        <v>45568.537837905096</v>
+      </c>
+      <c r="B191" s="8" t="s">
+        <v>566</v>
+      </c>
+      <c r="C191" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D191" s="8">
+        <v>20242340</v>
+      </c>
+      <c r="E191" s="8" t="s">
+        <v>567</v>
+      </c>
+      <c r="F191" s="8">
+        <v>3</v>
+      </c>
+      <c r="G191" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H191" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I191" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J191" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K191" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L191" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M191" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N191" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O191" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P191" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q191" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R191" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S191" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T191" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U191" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V191" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W191" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X191" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y191" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z191" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA191" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB191" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC191" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD191" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="192" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A192" s="4">
+        <v>45568.543277337958</v>
+      </c>
+      <c r="B192" s="5" t="s">
+        <v>568</v>
+      </c>
+      <c r="C192" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="D192" s="5">
+        <v>20192366</v>
+      </c>
+      <c r="E192" s="5" t="s">
+        <v>569</v>
+      </c>
+      <c r="F192" s="5">
+        <v>3</v>
+      </c>
+      <c r="G192" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="H192" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I192" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J192" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K192" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L192" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M192" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N192" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O192" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P192" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q192" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R192" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S192" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T192" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U192" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V192" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W192" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X192" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y192" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z192" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA192" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB192" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC192" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD192" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="193" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A193" s="7">
+        <v>45568.560783252316</v>
+      </c>
+      <c r="B193" s="8" t="s">
+        <v>570</v>
+      </c>
+      <c r="C193" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="D193" s="8">
+        <v>20246639</v>
+      </c>
+      <c r="E193" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="F193" s="8">
+        <v>3</v>
+      </c>
+      <c r="G193" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H193" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I193" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J193" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K193" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L193" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M193" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N193" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O193" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P193" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q193" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R193" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="S193" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T193" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="U193" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V193" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W193" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="X193" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y193" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z193" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA193" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB193" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC193" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD193" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="194" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A194" s="4">
+        <v>45568.568350567133</v>
+      </c>
+      <c r="B194" s="5" t="s">
+        <v>572</v>
+      </c>
+      <c r="C194" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="D194" s="5">
+        <v>20242227</v>
+      </c>
+      <c r="E194" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="F194" s="5">
+        <v>3</v>
+      </c>
+      <c r="G194" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H194" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I194" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J194" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K194" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L194" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M194" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N194" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O194" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P194" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q194" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R194" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S194" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T194" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U194" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V194" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W194" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X194" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y194" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z194" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA194" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB194" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC194" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD194" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="195" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A195" s="7">
+        <v>45568.582284490738</v>
+      </c>
+      <c r="B195" s="8" t="s">
+        <v>574</v>
+      </c>
+      <c r="C195" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D195" s="8">
+        <v>20242525</v>
+      </c>
+      <c r="E195" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="F195" s="8">
+        <v>3</v>
+      </c>
+      <c r="G195" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H195" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I195" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J195" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K195" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L195" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M195" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N195" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O195" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P195" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q195" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R195" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S195" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T195" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U195" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V195" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W195" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X195" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y195" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z195" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA195" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB195" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC195" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD195" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="196" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A196" s="4">
+        <v>45568.588117754625</v>
+      </c>
+      <c r="B196" s="5" t="s">
+        <v>575</v>
+      </c>
+      <c r="C196" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D196" s="5">
+        <v>20243801</v>
+      </c>
+      <c r="E196" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="F196" s="5">
+        <v>3</v>
+      </c>
+      <c r="G196" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H196" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I196" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J196" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K196" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="L196" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M196" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N196" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O196" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P196" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q196" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R196" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S196" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T196" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U196" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V196" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W196" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X196" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y196" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z196" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA196" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB196" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC196" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD196" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="197" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A197" s="7">
+        <v>45568.590303287041</v>
+      </c>
+      <c r="B197" s="8" t="s">
+        <v>577</v>
+      </c>
+      <c r="C197" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="D197" s="8">
+        <v>20235179</v>
+      </c>
+      <c r="E197" s="8" t="s">
+        <v>578</v>
+      </c>
+      <c r="F197" s="8">
+        <v>3</v>
+      </c>
+      <c r="G197" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H197" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I197" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J197" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K197" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L197" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M197" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N197" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O197" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P197" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q197" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R197" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S197" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T197" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U197" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V197" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W197" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="X197" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y197" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z197" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA197" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB197" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC197" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD197" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="198" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A198" s="4">
+        <v>45568.617451863422</v>
+      </c>
+      <c r="B198" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="C198" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D198" s="5">
+        <v>20246206</v>
+      </c>
+      <c r="E198" s="5" t="s">
+        <v>580</v>
+      </c>
+      <c r="F198" s="5">
+        <v>3</v>
+      </c>
+      <c r="G198" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H198" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I198" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J198" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K198" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L198" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M198" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N198" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O198" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P198" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q198" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R198" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S198" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T198" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U198" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V198" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W198" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X198" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y198" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z198" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA198" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB198" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC198" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD198" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="199" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A199" s="7">
+        <v>45568.638023020831</v>
+      </c>
+      <c r="B199" s="8" t="s">
+        <v>581</v>
+      </c>
+      <c r="C199" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D199" s="8">
+        <v>20214104</v>
+      </c>
+      <c r="E199" s="8" t="s">
+        <v>582</v>
+      </c>
+      <c r="F199" s="8">
+        <v>3</v>
+      </c>
+      <c r="G199" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H199" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I199" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J199" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K199" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L199" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M199" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N199" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O199" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P199" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q199" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R199" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S199" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T199" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U199" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V199" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W199" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X199" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y199" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z199" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA199" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB199" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC199" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD199" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="200" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A200" s="4">
+        <v>45568.643226446758</v>
+      </c>
+      <c r="B200" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="C200" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D200" s="5">
+        <v>20242736</v>
+      </c>
+      <c r="E200" s="5" t="s">
+        <v>584</v>
+      </c>
+      <c r="F200" s="5">
+        <v>3</v>
+      </c>
+      <c r="G200" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H200" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I200" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J200" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K200" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L200" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M200" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N200" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O200" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="P200" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q200" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R200" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S200" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T200" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U200" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V200" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W200" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="X200" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y200" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z200" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA200" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB200" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC200" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD200" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="201" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A201" s="7">
+        <v>45568.685352523149</v>
+      </c>
+      <c r="B201" s="8" t="s">
+        <v>585</v>
+      </c>
+      <c r="C201" s="8" t="s">
+        <v>586</v>
+      </c>
+      <c r="D201" s="8">
+        <v>20201007</v>
+      </c>
+      <c r="E201" s="8" t="s">
+        <v>587</v>
+      </c>
+      <c r="F201" s="8">
+        <v>3</v>
+      </c>
+      <c r="G201" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H201" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I201" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J201" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="K201" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L201" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M201" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N201" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O201" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P201" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q201" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="R201" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S201" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T201" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U201" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V201" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W201" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X201" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y201" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z201" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA201" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB201" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC201" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD201" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="202" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A202" s="4">
+        <v>45568.694490451388</v>
+      </c>
+      <c r="B202" s="5" t="s">
+        <v>588</v>
+      </c>
+      <c r="C202" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D202" s="5">
+        <v>20246248</v>
+      </c>
+      <c r="E202" s="5" t="s">
+        <v>589</v>
+      </c>
+      <c r="F202" s="5">
+        <v>3</v>
+      </c>
+      <c r="G202" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H202" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I202" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J202" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K202" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L202" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M202" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N202" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O202" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P202" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q202" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R202" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S202" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T202" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U202" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V202" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W202" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X202" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y202" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z202" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA202" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB202" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC202" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD202" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="203" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A203" s="7">
+        <v>45568.706669675928</v>
+      </c>
+      <c r="B203" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="C203" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="D203" s="8">
+        <v>20192560</v>
+      </c>
+      <c r="E203" s="8" t="s">
+        <v>591</v>
+      </c>
+      <c r="F203" s="8">
+        <v>3</v>
+      </c>
+      <c r="G203" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H203" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I203" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J203" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K203" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L203" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M203" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N203" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O203" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P203" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q203" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R203" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S203" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T203" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U203" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V203" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W203" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X203" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y203" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z203" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA203" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB203" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC203" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD203" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="204" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A204" s="4">
+        <v>45568.71200594907</v>
+      </c>
+      <c r="B204" s="5" t="s">
+        <v>592</v>
+      </c>
+      <c r="C204" s="5" t="s">
+        <v>586</v>
+      </c>
+      <c r="D204" s="5">
+        <v>20221005</v>
+      </c>
+      <c r="E204" s="5" t="s">
+        <v>593</v>
+      </c>
+      <c r="F204" s="5">
+        <v>3</v>
+      </c>
+      <c r="G204" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H204" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I204" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J204" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K204" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L204" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M204" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N204" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O204" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P204" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q204" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R204" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S204" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T204" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U204" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V204" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W204" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X204" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y204" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z204" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA204" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB204" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC204" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD204" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="205" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A205" s="7">
+        <v>45568.716963877319</v>
+      </c>
+      <c r="B205" s="8" t="s">
+        <v>594</v>
+      </c>
+      <c r="C205" s="8" t="s">
+        <v>595</v>
+      </c>
+      <c r="D205" s="8">
+        <v>20241204</v>
+      </c>
+      <c r="E205" s="8" t="s">
+        <v>596</v>
+      </c>
+      <c r="F205" s="8">
+        <v>3</v>
+      </c>
+      <c r="G205" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H205" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I205" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J205" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K205" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L205" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M205" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="N205" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O205" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P205" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q205" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R205" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S205" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T205" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="U205" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V205" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="W205" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X205" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y205" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z205" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA205" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB205" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC205" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD205" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="206" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A206" s="4">
+        <v>45568.71800680556</v>
+      </c>
+      <c r="B206" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="C206" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D206" s="5">
+        <v>20235210</v>
+      </c>
+      <c r="E206" s="5" t="s">
+        <v>598</v>
+      </c>
+      <c r="F206" s="5">
+        <v>3</v>
+      </c>
+      <c r="G206" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H206" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I206" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J206" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K206" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L206" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M206" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N206" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O206" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P206" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q206" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R206" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S206" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T206" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="U206" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V206" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W206" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X206" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y206" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z206" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA206" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB206" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC206" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD206" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="207" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A207" s="13">
+        <v>45568.743135578705</v>
+      </c>
+      <c r="B207" s="14" t="s">
+        <v>599</v>
+      </c>
+      <c r="C207" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D207" s="14">
+        <v>20192936</v>
+      </c>
+      <c r="E207" s="14" t="s">
+        <v>600</v>
+      </c>
+      <c r="F207" s="14">
+        <v>3</v>
+      </c>
+      <c r="G207" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="H207" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="I207" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J207" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="K207" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="L207" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="M207" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N207" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="O207" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P207" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q207" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="R207" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="S207" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="T207" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="U207" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="V207" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="W207" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="X207" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y207" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z207" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA207" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB207" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC207" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD207" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
literacy, 240930 modified 5
</commit_message>
<xml_diff>
--- a/R/data/literacy_240930.xlsx
+++ b/R/data/literacy_240930.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6AB34EE-90B2-E747-89E4-5665D308EC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA953287-6DDF-C547-AD8B-046116B3B8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50400" yWindow="1360" windowWidth="44800" windowHeight="24700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5592" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6132" uniqueCount="641">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -1823,6 +1823,126 @@
   </si>
   <si>
     <t>이동기</t>
+  </si>
+  <si>
+    <t>0223wltn@naver.com</t>
+  </si>
+  <si>
+    <t>홍지수</t>
+  </si>
+  <si>
+    <t>donghyun6652@gmail.com</t>
+  </si>
+  <si>
+    <t>한동현</t>
+  </si>
+  <si>
+    <t>ckswo00@gmail.com</t>
+  </si>
+  <si>
+    <t>이찬재</t>
+  </si>
+  <si>
+    <t>dongkyolee@naver.com</t>
+  </si>
+  <si>
+    <t>이동교</t>
+  </si>
+  <si>
+    <t>anfytrltk3@naver.com</t>
+  </si>
+  <si>
+    <t>윤가영</t>
+  </si>
+  <si>
+    <t>sally200408@gmail.com</t>
+  </si>
+  <si>
+    <t>박경화</t>
+  </si>
+  <si>
+    <t>kyg031988@gmail.com</t>
+  </si>
+  <si>
+    <t>김윤겸</t>
+  </si>
+  <si>
+    <t>bagminhyeog534@gmail.com</t>
+  </si>
+  <si>
+    <t>박민혁</t>
+  </si>
+  <si>
+    <t>snp040609@naver.com</t>
+  </si>
+  <si>
+    <t>박세나</t>
+  </si>
+  <si>
+    <t>wizkids0418@naver.com</t>
+  </si>
+  <si>
+    <t>박혜인</t>
+  </si>
+  <si>
+    <t>ilylive999@gmail.com</t>
+  </si>
+  <si>
+    <t>이가현</t>
+  </si>
+  <si>
+    <t>qwe92517@gmail.com</t>
+  </si>
+  <si>
+    <t>이진영</t>
+  </si>
+  <si>
+    <t>ujs4198@naver.com</t>
+  </si>
+  <si>
+    <t>엄준식</t>
+  </si>
+  <si>
+    <t>nyj7013@naver.com</t>
+  </si>
+  <si>
+    <t>노예진</t>
+  </si>
+  <si>
+    <t>efgh124@naver.com</t>
+  </si>
+  <si>
+    <t>정윤서</t>
+  </si>
+  <si>
+    <t>yohihong@gmail.com</t>
+  </si>
+  <si>
+    <t>민홍기</t>
+  </si>
+  <si>
+    <t>msy123581@naver.com</t>
+  </si>
+  <si>
+    <t>문신영</t>
+  </si>
+  <si>
+    <t>leejhzzang2005@naver.com</t>
+  </si>
+  <si>
+    <t>이주현</t>
+  </si>
+  <si>
+    <t>minwl19@naver.com</t>
+  </si>
+  <si>
+    <t>조민지</t>
+  </si>
+  <si>
+    <t>bagj11533@gmail.com</t>
+  </si>
+  <si>
+    <t>박준형</t>
   </si>
 </sst>
 </file>
@@ -2237,7 +2357,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:AD207">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:AD227">
   <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -2475,11 +2595,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD207"/>
+  <dimension ref="A1:AD227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D221" sqref="D221"/>
+      <selection pane="bottomLeft" activeCell="E239" sqref="E239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -21556,6 +21676,1846 @@
         <v>56</v>
       </c>
     </row>
+    <row r="208" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A208" s="4">
+        <v>45568.789632418979</v>
+      </c>
+      <c r="B208" s="5" t="s">
+        <v>601</v>
+      </c>
+      <c r="C208" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D208" s="5">
+        <v>20243850</v>
+      </c>
+      <c r="E208" s="5" t="s">
+        <v>602</v>
+      </c>
+      <c r="F208" s="5">
+        <v>3</v>
+      </c>
+      <c r="G208" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H208" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I208" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J208" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K208" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L208" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M208" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N208" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O208" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P208" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q208" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R208" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S208" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T208" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="U208" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V208" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W208" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X208" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y208" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z208" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA208" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB208" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC208" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD208" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="209" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A209" s="7">
+        <v>45568.803411840279</v>
+      </c>
+      <c r="B209" s="8" t="s">
+        <v>603</v>
+      </c>
+      <c r="C209" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D209" s="8">
+        <v>20246300</v>
+      </c>
+      <c r="E209" s="8" t="s">
+        <v>604</v>
+      </c>
+      <c r="F209" s="8">
+        <v>3</v>
+      </c>
+      <c r="G209" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H209" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I209" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J209" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K209" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L209" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M209" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N209" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O209" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P209" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q209" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R209" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S209" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T209" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="U209" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V209" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W209" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X209" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y209" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z209" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA209" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB209" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC209" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD209" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="210" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A210" s="4">
+        <v>45568.804496956014</v>
+      </c>
+      <c r="B210" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="C210" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="D210" s="5">
+        <v>20217151</v>
+      </c>
+      <c r="E210" s="5" t="s">
+        <v>606</v>
+      </c>
+      <c r="F210" s="5">
+        <v>2</v>
+      </c>
+      <c r="G210" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="H210" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I210" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J210" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="K210" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L210" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M210" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="N210" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="O210" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="P210" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q210" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R210" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="S210" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="T210" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="U210" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="V210" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="W210" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X210" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="Y210" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z210" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AA210" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB210" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC210" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD210" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="211" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A211" s="7">
+        <v>45568.861559131939</v>
+      </c>
+      <c r="B211" s="8" t="s">
+        <v>607</v>
+      </c>
+      <c r="C211" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="D211" s="8">
+        <v>20213241</v>
+      </c>
+      <c r="E211" s="8" t="s">
+        <v>608</v>
+      </c>
+      <c r="F211" s="8">
+        <v>3</v>
+      </c>
+      <c r="G211" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H211" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I211" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J211" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K211" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="L211" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M211" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N211" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O211" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P211" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q211" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R211" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S211" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T211" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="U211" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V211" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W211" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X211" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y211" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z211" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA211" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB211" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC211" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD211" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="212" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A212" s="4">
+        <v>45568.862717673612</v>
+      </c>
+      <c r="B212" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="C212" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D212" s="5">
+        <v>20243830</v>
+      </c>
+      <c r="E212" s="5" t="s">
+        <v>610</v>
+      </c>
+      <c r="F212" s="5">
+        <v>3</v>
+      </c>
+      <c r="G212" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H212" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I212" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J212" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K212" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="L212" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M212" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N212" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O212" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P212" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q212" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R212" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S212" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T212" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U212" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V212" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W212" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X212" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y212" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z212" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA212" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB212" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC212" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD212" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="213" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A213" s="7">
+        <v>45568.869324166662</v>
+      </c>
+      <c r="B213" s="8" t="s">
+        <v>611</v>
+      </c>
+      <c r="C213" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D213" s="8">
+        <v>20212818</v>
+      </c>
+      <c r="E213" s="8" t="s">
+        <v>612</v>
+      </c>
+      <c r="F213" s="8">
+        <v>3</v>
+      </c>
+      <c r="G213" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H213" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I213" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J213" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K213" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L213" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M213" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N213" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O213" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P213" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q213" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R213" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S213" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T213" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U213" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V213" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W213" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X213" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y213" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z213" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA213" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB213" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC213" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD213" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="214" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A214" s="4">
+        <v>45568.890650023153</v>
+      </c>
+      <c r="B214" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="C214" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D214" s="5">
+        <v>20231606</v>
+      </c>
+      <c r="E214" s="5" t="s">
+        <v>614</v>
+      </c>
+      <c r="F214" s="5">
+        <v>3</v>
+      </c>
+      <c r="G214" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H214" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I214" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J214" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="K214" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L214" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M214" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N214" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O214" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P214" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q214" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R214" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S214" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T214" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U214" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="V214" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W214" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X214" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y214" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z214" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA214" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB214" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC214" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD214" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="215" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A215" s="7">
+        <v>45568.930487569443</v>
+      </c>
+      <c r="B215" s="8" t="s">
+        <v>615</v>
+      </c>
+      <c r="C215" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="D215" s="8">
+        <v>20242320</v>
+      </c>
+      <c r="E215" s="8" t="s">
+        <v>616</v>
+      </c>
+      <c r="F215" s="8">
+        <v>3</v>
+      </c>
+      <c r="G215" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="H215" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I215" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J215" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K215" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L215" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M215" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N215" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O215" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P215" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q215" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R215" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S215" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="T215" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U215" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V215" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W215" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X215" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y215" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z215" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA215" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB215" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC215" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD215" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="216" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A216" s="4">
+        <v>45568.990932488421</v>
+      </c>
+      <c r="B216" s="5" t="s">
+        <v>617</v>
+      </c>
+      <c r="C216" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D216" s="5">
+        <v>20242957</v>
+      </c>
+      <c r="E216" s="5" t="s">
+        <v>618</v>
+      </c>
+      <c r="F216" s="5">
+        <v>3</v>
+      </c>
+      <c r="G216" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H216" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I216" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J216" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K216" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L216" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M216" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N216" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O216" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P216" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q216" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R216" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S216" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T216" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U216" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V216" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W216" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X216" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y216" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z216" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA216" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB216" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC216" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD216" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="217" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A217" s="7">
+        <v>45569.006115034717</v>
+      </c>
+      <c r="B217" s="8" t="s">
+        <v>619</v>
+      </c>
+      <c r="C217" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D217" s="8">
+        <v>20242427</v>
+      </c>
+      <c r="E217" s="8" t="s">
+        <v>620</v>
+      </c>
+      <c r="F217" s="8">
+        <v>3</v>
+      </c>
+      <c r="G217" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H217" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I217" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J217" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K217" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L217" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M217" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N217" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O217" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P217" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q217" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R217" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S217" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T217" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="U217" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V217" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W217" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X217" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y217" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z217" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA217" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB217" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC217" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD217" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="218" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A218" s="4">
+        <v>45569.023525879631</v>
+      </c>
+      <c r="B218" s="5" t="s">
+        <v>621</v>
+      </c>
+      <c r="C218" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D218" s="5">
+        <v>20231621</v>
+      </c>
+      <c r="E218" s="5" t="s">
+        <v>622</v>
+      </c>
+      <c r="F218" s="5">
+        <v>3</v>
+      </c>
+      <c r="G218" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H218" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I218" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J218" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K218" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L218" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M218" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N218" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O218" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P218" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q218" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R218" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S218" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T218" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="U218" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="V218" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W218" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="X218" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y218" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z218" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA218" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB218" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC218" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD218" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="219" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A219" s="7">
+        <v>45569.032233217593</v>
+      </c>
+      <c r="B219" s="8" t="s">
+        <v>623</v>
+      </c>
+      <c r="C219" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D219" s="8">
+        <v>20246271</v>
+      </c>
+      <c r="E219" s="8" t="s">
+        <v>624</v>
+      </c>
+      <c r="F219" s="8">
+        <v>3</v>
+      </c>
+      <c r="G219" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H219" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I219" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J219" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K219" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L219" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M219" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N219" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O219" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P219" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q219" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R219" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S219" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T219" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="U219" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V219" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W219" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X219" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y219" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z219" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA219" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB219" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC219" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD219" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="220" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A220" s="4">
+        <v>45569.040550381949</v>
+      </c>
+      <c r="B220" s="5" t="s">
+        <v>625</v>
+      </c>
+      <c r="C220" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D220" s="5">
+        <v>20197118</v>
+      </c>
+      <c r="E220" s="5" t="s">
+        <v>626</v>
+      </c>
+      <c r="F220" s="5">
+        <v>3</v>
+      </c>
+      <c r="G220" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H220" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I220" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J220" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K220" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L220" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M220" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N220" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O220" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P220" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q220" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R220" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S220" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T220" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U220" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V220" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W220" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X220" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y220" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z220" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA220" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB220" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC220" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD220" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="221" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A221" s="7">
+        <v>45569.048287488426</v>
+      </c>
+      <c r="B221" s="8" t="s">
+        <v>627</v>
+      </c>
+      <c r="C221" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D221" s="8">
+        <v>20246235</v>
+      </c>
+      <c r="E221" s="8" t="s">
+        <v>628</v>
+      </c>
+      <c r="F221" s="8">
+        <v>3</v>
+      </c>
+      <c r="G221" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H221" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I221" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J221" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K221" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="L221" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M221" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N221" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O221" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P221" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q221" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R221" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S221" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T221" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U221" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="V221" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W221" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X221" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y221" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z221" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA221" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB221" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC221" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD221" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="222" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A222" s="4">
+        <v>45569.052534537041</v>
+      </c>
+      <c r="B222" s="5" t="s">
+        <v>629</v>
+      </c>
+      <c r="C222" s="5" t="s">
+        <v>519</v>
+      </c>
+      <c r="D222" s="5">
+        <v>20246282</v>
+      </c>
+      <c r="E222" s="5" t="s">
+        <v>630</v>
+      </c>
+      <c r="F222" s="5">
+        <v>3</v>
+      </c>
+      <c r="G222" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H222" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I222" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J222" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K222" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L222" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M222" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N222" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O222" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P222" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q222" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R222" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S222" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T222" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="U222" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V222" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W222" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X222" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y222" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z222" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA222" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB222" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC222" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD222" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="223" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A223" s="7">
+        <v>45569.057582893518</v>
+      </c>
+      <c r="B223" s="8" t="s">
+        <v>631</v>
+      </c>
+      <c r="C223" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D223" s="8">
+        <v>20245161</v>
+      </c>
+      <c r="E223" s="8" t="s">
+        <v>632</v>
+      </c>
+      <c r="F223" s="8">
+        <v>3</v>
+      </c>
+      <c r="G223" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H223" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I223" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J223" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K223" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L223" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M223" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N223" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O223" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P223" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q223" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R223" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S223" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T223" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="U223" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V223" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W223" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X223" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y223" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z223" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA223" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB223" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC223" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD223" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="224" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A224" s="4">
+        <v>45569.075522175925</v>
+      </c>
+      <c r="B224" s="5" t="s">
+        <v>633</v>
+      </c>
+      <c r="C224" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="D224" s="5">
+        <v>20241519</v>
+      </c>
+      <c r="E224" s="5" t="s">
+        <v>634</v>
+      </c>
+      <c r="F224" s="5">
+        <v>3</v>
+      </c>
+      <c r="G224" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H224" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I224" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J224" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="K224" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="L224" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M224" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N224" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O224" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P224" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q224" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R224" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S224" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T224" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U224" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V224" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W224" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X224" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y224" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z224" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA224" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB224" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC224" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD224" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="225" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A225" s="7">
+        <v>45569.076920104169</v>
+      </c>
+      <c r="B225" s="8" t="s">
+        <v>635</v>
+      </c>
+      <c r="C225" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D225" s="8">
+        <v>20242342</v>
+      </c>
+      <c r="E225" s="8" t="s">
+        <v>636</v>
+      </c>
+      <c r="F225" s="8">
+        <v>3</v>
+      </c>
+      <c r="G225" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H225" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I225" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J225" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K225" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L225" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M225" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N225" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O225" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P225" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q225" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R225" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S225" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T225" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U225" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V225" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W225" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X225" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y225" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z225" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA225" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB225" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC225" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD225" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="226" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A226" s="4">
+        <v>45569.088212974537</v>
+      </c>
+      <c r="B226" s="5" t="s">
+        <v>637</v>
+      </c>
+      <c r="C226" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="D226" s="5">
+        <v>20217178</v>
+      </c>
+      <c r="E226" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="F226" s="5">
+        <v>3</v>
+      </c>
+      <c r="G226" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H226" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I226" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J226" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K226" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L226" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M226" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N226" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O226" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P226" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q226" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R226" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S226" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T226" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U226" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V226" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W226" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X226" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y226" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z226" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA226" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB226" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC226" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD226" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="227" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A227" s="13">
+        <v>45569.245331666665</v>
+      </c>
+      <c r="B227" s="14" t="s">
+        <v>639</v>
+      </c>
+      <c r="C227" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="D227" s="14">
+        <v>24</v>
+      </c>
+      <c r="E227" s="14" t="s">
+        <v>640</v>
+      </c>
+      <c r="F227" s="14">
+        <v>3</v>
+      </c>
+      <c r="G227" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="H227" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="I227" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J227" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="K227" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="L227" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="M227" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N227" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="O227" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P227" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q227" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="R227" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="S227" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="T227" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="U227" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="V227" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="W227" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="X227" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y227" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z227" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA227" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB227" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="AC227" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD227" s="15" t="s">
+        <v>214</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
literacy, 240930 modified 6
</commit_message>
<xml_diff>
--- a/R/data/literacy_240930.xlsx
+++ b/R/data/literacy_240930.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA953287-6DDF-C547-AD8B-046116B3B8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC2A6E9-ED0F-244E-A46D-039A7155B195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50400" yWindow="1360" windowWidth="44800" windowHeight="24700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6132" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6834" uniqueCount="695">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -1943,6 +1943,168 @@
   </si>
   <si>
     <t>박준형</t>
+  </si>
+  <si>
+    <t>bvc023@naver.com</t>
+  </si>
+  <si>
+    <t>김수영</t>
+  </si>
+  <si>
+    <t>ginny1024@naver.com</t>
+  </si>
+  <si>
+    <t>김희원</t>
+  </si>
+  <si>
+    <t>znfh527gkfn@naver.com</t>
+  </si>
+  <si>
+    <t>조준연</t>
+  </si>
+  <si>
+    <t>h20241207@glab.hallym.ac.kr</t>
+  </si>
+  <si>
+    <t>문소정</t>
+  </si>
+  <si>
+    <t>kjinju0518@naver.com</t>
+  </si>
+  <si>
+    <t>김진주</t>
+  </si>
+  <si>
+    <t>0616sdh@naver.com</t>
+  </si>
+  <si>
+    <t>신동현</t>
+  </si>
+  <si>
+    <t>a01051265769@gmail.com</t>
+  </si>
+  <si>
+    <t>안현영</t>
+  </si>
+  <si>
+    <t>bevery2685@gmail.com</t>
+  </si>
+  <si>
+    <t>반도체디스플레이</t>
+  </si>
+  <si>
+    <t>조영태</t>
+  </si>
+  <si>
+    <t>yoonbin0304@naver.com</t>
+  </si>
+  <si>
+    <t>최윤빈</t>
+  </si>
+  <si>
+    <t>rlaehdnr999@naver.com</t>
+  </si>
+  <si>
+    <t>김도욱</t>
+  </si>
+  <si>
+    <t>chorok052150@naver.com</t>
+  </si>
+  <si>
+    <t>김미니</t>
+  </si>
+  <si>
+    <t>06kongkongsoon@gmail.com</t>
+  </si>
+  <si>
+    <t>이서연</t>
+  </si>
+  <si>
+    <t>ddoyeong0509@gmail.com</t>
+  </si>
+  <si>
+    <t>윤소영</t>
+  </si>
+  <si>
+    <t>jhue0901@gmail.com</t>
+  </si>
+  <si>
+    <t>글로벌비지니스학과</t>
+  </si>
+  <si>
+    <t>전하율</t>
+  </si>
+  <si>
+    <t>leenara633@gamil.com</t>
+  </si>
+  <si>
+    <t>이나라</t>
+  </si>
+  <si>
+    <t>sangim041113@gmail.com</t>
+  </si>
+  <si>
+    <t>용상임</t>
+  </si>
+  <si>
+    <t>byl0730@naver.com</t>
+  </si>
+  <si>
+    <t>변예림</t>
+  </si>
+  <si>
+    <t>aj7082331@gmail.com</t>
+  </si>
+  <si>
+    <t>조아나</t>
+  </si>
+  <si>
+    <t>sojunghanbomul@gmail.com</t>
+  </si>
+  <si>
+    <t>김상준</t>
+  </si>
+  <si>
+    <t>yssong1919@naver.com</t>
+  </si>
+  <si>
+    <t>송예상</t>
+  </si>
+  <si>
+    <t>cobas67@naver.com</t>
+  </si>
+  <si>
+    <t>스마트iot</t>
+  </si>
+  <si>
+    <t>박근혁</t>
+  </si>
+  <si>
+    <t>swncelt@naver.com</t>
+  </si>
+  <si>
+    <t>박은서</t>
+  </si>
+  <si>
+    <t>yumi0901gami@gmail.com</t>
+  </si>
+  <si>
+    <t>4080jjh@gmail.com</t>
+  </si>
+  <si>
+    <t>장재환</t>
+  </si>
+  <si>
+    <t>obbobb7@gmail.com</t>
+  </si>
+  <si>
+    <t>구재영</t>
+  </si>
+  <si>
+    <t>t01094887068@gmail.com</t>
+  </si>
+  <si>
+    <t>손민재</t>
   </si>
 </sst>
 </file>
@@ -2357,7 +2519,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:AD227">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:AD253">
   <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -2595,11 +2757,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD227"/>
+  <dimension ref="A1:AD253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E239" sqref="E239"/>
+      <selection pane="bottomLeft" activeCell="E255" sqref="E255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -23516,6 +23678,2398 @@
         <v>214</v>
       </c>
     </row>
+    <row r="228" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A228" s="4">
+        <v>45569.407633935189</v>
+      </c>
+      <c r="B228" s="5" t="s">
+        <v>641</v>
+      </c>
+      <c r="C228" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="D228" s="5">
+        <v>20217035</v>
+      </c>
+      <c r="E228" s="5" t="s">
+        <v>642</v>
+      </c>
+      <c r="F228" s="5">
+        <v>3</v>
+      </c>
+      <c r="G228" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H228" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I228" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J228" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K228" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L228" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M228" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N228" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O228" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P228" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q228" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R228" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S228" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T228" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U228" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V228" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W228" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X228" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y228" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z228" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA228" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB228" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC228" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD228" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="229" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A229" s="7">
+        <v>45569.409270902775</v>
+      </c>
+      <c r="B229" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="C229" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D229" s="8">
+        <v>20246233</v>
+      </c>
+      <c r="E229" s="8" t="s">
+        <v>644</v>
+      </c>
+      <c r="F229" s="8">
+        <v>3</v>
+      </c>
+      <c r="G229" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H229" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I229" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J229" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K229" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L229" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M229" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N229" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O229" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P229" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q229" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R229" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S229" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T229" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U229" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V229" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W229" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X229" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y229" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z229" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA229" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB229" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC229" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD229" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="230" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A230" s="4">
+        <v>45569.417845312499</v>
+      </c>
+      <c r="B230" s="5" t="s">
+        <v>645</v>
+      </c>
+      <c r="C230" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D230" s="5">
+        <v>20222359</v>
+      </c>
+      <c r="E230" s="5" t="s">
+        <v>646</v>
+      </c>
+      <c r="F230" s="5">
+        <v>3</v>
+      </c>
+      <c r="G230" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H230" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I230" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J230" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K230" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L230" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M230" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N230" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O230" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P230" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q230" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R230" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S230" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T230" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U230" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V230" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="W230" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X230" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y230" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z230" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA230" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB230" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC230" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD230" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="231" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A231" s="7">
+        <v>45569.500130625005</v>
+      </c>
+      <c r="B231" s="8" t="s">
+        <v>647</v>
+      </c>
+      <c r="C231" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="D231" s="8">
+        <v>20241207</v>
+      </c>
+      <c r="E231" s="8" t="s">
+        <v>648</v>
+      </c>
+      <c r="F231" s="8">
+        <v>3</v>
+      </c>
+      <c r="G231" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H231" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I231" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J231" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K231" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L231" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M231" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N231" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O231" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P231" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q231" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R231" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S231" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T231" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U231" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V231" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W231" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X231" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y231" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z231" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA231" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB231" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC231" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD231" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="232" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A232" s="4">
+        <v>45569.505158877313</v>
+      </c>
+      <c r="B232" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="C232" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D232" s="5">
+        <v>20232937</v>
+      </c>
+      <c r="E232" s="5" t="s">
+        <v>650</v>
+      </c>
+      <c r="F232" s="5">
+        <v>3</v>
+      </c>
+      <c r="G232" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H232" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I232" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J232" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K232" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L232" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M232" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N232" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O232" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P232" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q232" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R232" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S232" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T232" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U232" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V232" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W232" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X232" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y232" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z232" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA232" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB232" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC232" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD232" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="233" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A233" s="7">
+        <v>45569.517907488422</v>
+      </c>
+      <c r="B233" s="8" t="s">
+        <v>651</v>
+      </c>
+      <c r="C233" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D233" s="8">
+        <v>20202730</v>
+      </c>
+      <c r="E233" s="8" t="s">
+        <v>652</v>
+      </c>
+      <c r="F233" s="8">
+        <v>3</v>
+      </c>
+      <c r="G233" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H233" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I233" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J233" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K233" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="L233" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M233" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N233" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O233" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P233" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q233" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R233" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S233" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T233" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U233" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V233" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W233" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X233" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y233" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z233" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA233" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB233" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC233" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD233" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="234" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A234" s="4">
+        <v>45569.607134664351</v>
+      </c>
+      <c r="B234" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="C234" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="D234" s="5">
+        <v>20243414</v>
+      </c>
+      <c r="E234" s="5" t="s">
+        <v>654</v>
+      </c>
+      <c r="F234" s="5">
+        <v>3</v>
+      </c>
+      <c r="G234" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H234" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I234" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J234" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K234" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L234" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="M234" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N234" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O234" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P234" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q234" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R234" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S234" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T234" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U234" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V234" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W234" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X234" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y234" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z234" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA234" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB234" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC234" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD234" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="235" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A235" s="7">
+        <v>45569.648270185186</v>
+      </c>
+      <c r="B235" s="8" t="s">
+        <v>655</v>
+      </c>
+      <c r="C235" s="8" t="s">
+        <v>656</v>
+      </c>
+      <c r="D235" s="8">
+        <v>20243354</v>
+      </c>
+      <c r="E235" s="8" t="s">
+        <v>657</v>
+      </c>
+      <c r="F235" s="8">
+        <v>3</v>
+      </c>
+      <c r="G235" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H235" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I235" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J235" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K235" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L235" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M235" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="N235" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O235" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P235" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q235" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R235" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="S235" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="T235" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="U235" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V235" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W235" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X235" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y235" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z235" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA235" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB235" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC235" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD235" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="236" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A236" s="4">
+        <v>45569.658737060185</v>
+      </c>
+      <c r="B236" s="5" t="s">
+        <v>658</v>
+      </c>
+      <c r="C236" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D236" s="5">
+        <v>20242138</v>
+      </c>
+      <c r="E236" s="5" t="s">
+        <v>659</v>
+      </c>
+      <c r="F236" s="5">
+        <v>3</v>
+      </c>
+      <c r="G236" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H236" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I236" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J236" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K236" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="L236" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M236" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N236" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O236" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P236" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q236" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R236" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S236" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T236" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U236" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V236" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="W236" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X236" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y236" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z236" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA236" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB236" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC236" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD236" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="237" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A237" s="7">
+        <v>45569.668222372682</v>
+      </c>
+      <c r="B237" s="8" t="s">
+        <v>660</v>
+      </c>
+      <c r="C237" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D237" s="8">
+        <v>20221007</v>
+      </c>
+      <c r="E237" s="8" t="s">
+        <v>661</v>
+      </c>
+      <c r="F237" s="8">
+        <v>3</v>
+      </c>
+      <c r="G237" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H237" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I237" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J237" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K237" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L237" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M237" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N237" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O237" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P237" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q237" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R237" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S237" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T237" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="U237" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V237" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W237" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X237" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y237" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z237" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA237" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB237" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC237" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD237" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="238" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A238" s="4">
+        <v>45569.671258113427</v>
+      </c>
+      <c r="B238" s="5" t="s">
+        <v>662</v>
+      </c>
+      <c r="C238" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D238" s="5">
+        <v>20242307</v>
+      </c>
+      <c r="E238" s="5" t="s">
+        <v>663</v>
+      </c>
+      <c r="F238" s="5">
+        <v>3</v>
+      </c>
+      <c r="G238" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H238" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I238" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J238" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K238" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L238" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M238" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N238" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O238" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P238" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q238" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R238" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S238" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T238" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U238" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V238" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W238" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X238" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y238" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z238" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA238" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB238" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC238" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD238" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="239" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A239" s="7">
+        <v>45569.672888229165</v>
+      </c>
+      <c r="B239" s="8" t="s">
+        <v>664</v>
+      </c>
+      <c r="C239" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D239" s="8">
+        <v>20242732</v>
+      </c>
+      <c r="E239" s="8" t="s">
+        <v>665</v>
+      </c>
+      <c r="F239" s="8">
+        <v>3</v>
+      </c>
+      <c r="G239" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H239" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I239" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J239" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K239" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L239" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M239" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N239" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O239" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P239" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q239" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R239" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S239" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T239" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="U239" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V239" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W239" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X239" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y239" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z239" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA239" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB239" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC239" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD239" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="240" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A240" s="4">
+        <v>45569.681496562502</v>
+      </c>
+      <c r="B240" s="5" t="s">
+        <v>666</v>
+      </c>
+      <c r="C240" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="D240" s="5">
+        <v>20242424</v>
+      </c>
+      <c r="E240" s="5" t="s">
+        <v>667</v>
+      </c>
+      <c r="F240" s="5">
+        <v>3</v>
+      </c>
+      <c r="G240" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H240" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I240" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J240" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K240" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L240" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M240" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N240" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O240" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P240" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q240" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R240" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S240" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T240" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U240" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V240" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W240" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X240" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y240" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z240" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA240" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB240" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC240" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD240" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="241" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A241" s="7">
+        <v>45569.695448321756</v>
+      </c>
+      <c r="B241" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C241" s="8" t="s">
+        <v>669</v>
+      </c>
+      <c r="D241" s="8">
+        <v>20246420</v>
+      </c>
+      <c r="E241" s="8" t="s">
+        <v>670</v>
+      </c>
+      <c r="F241" s="8">
+        <v>3</v>
+      </c>
+      <c r="G241" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H241" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I241" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J241" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K241" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L241" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M241" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N241" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O241" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P241" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q241" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R241" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S241" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T241" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U241" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V241" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W241" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X241" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y241" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z241" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA241" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB241" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC241" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD241" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="242" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A242" s="4">
+        <v>45569.732902951393</v>
+      </c>
+      <c r="B242" s="5" t="s">
+        <v>671</v>
+      </c>
+      <c r="C242" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D242" s="5">
+        <v>20241065</v>
+      </c>
+      <c r="E242" s="5" t="s">
+        <v>672</v>
+      </c>
+      <c r="F242" s="5">
+        <v>3</v>
+      </c>
+      <c r="G242" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="H242" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I242" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="J242" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K242" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L242" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M242" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="N242" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O242" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="P242" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q242" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R242" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="S242" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="T242" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U242" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="V242" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W242" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="X242" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y242" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z242" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA242" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB242" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC242" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="AD242" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="243" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A243" s="7">
+        <v>45569.74004827546</v>
+      </c>
+      <c r="B243" s="8" t="s">
+        <v>673</v>
+      </c>
+      <c r="C243" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D243" s="8">
+        <v>20235209</v>
+      </c>
+      <c r="E243" s="8" t="s">
+        <v>674</v>
+      </c>
+      <c r="F243" s="8">
+        <v>3</v>
+      </c>
+      <c r="G243" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H243" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I243" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J243" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K243" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L243" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M243" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N243" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O243" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P243" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q243" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R243" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S243" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T243" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U243" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V243" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W243" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X243" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y243" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z243" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA243" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB243" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC243" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD243" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="244" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A244" s="4">
+        <v>45569.750188622682</v>
+      </c>
+      <c r="B244" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="C244" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D244" s="5">
+        <v>20243715</v>
+      </c>
+      <c r="E244" s="5" t="s">
+        <v>676</v>
+      </c>
+      <c r="F244" s="5">
+        <v>3</v>
+      </c>
+      <c r="G244" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H244" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I244" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J244" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K244" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L244" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M244" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N244" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O244" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P244" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q244" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="R244" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S244" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T244" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="U244" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V244" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W244" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="X244" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y244" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z244" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA244" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB244" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC244" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD244" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="245" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A245" s="7">
+        <v>45569.792857199078</v>
+      </c>
+      <c r="B245" s="8" t="s">
+        <v>677</v>
+      </c>
+      <c r="C245" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D245" s="8">
+        <v>20233849</v>
+      </c>
+      <c r="E245" s="8" t="s">
+        <v>678</v>
+      </c>
+      <c r="F245" s="8">
+        <v>3</v>
+      </c>
+      <c r="G245" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H245" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I245" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J245" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K245" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L245" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M245" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N245" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O245" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P245" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q245" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R245" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S245" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T245" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U245" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V245" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W245" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X245" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y245" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z245" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA245" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB245" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC245" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD245" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="246" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A246" s="4">
+        <v>45569.817876273148</v>
+      </c>
+      <c r="B246" s="5" t="s">
+        <v>679</v>
+      </c>
+      <c r="C246" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="D246" s="5">
+        <v>20241513</v>
+      </c>
+      <c r="E246" s="5" t="s">
+        <v>680</v>
+      </c>
+      <c r="F246" s="5">
+        <v>3</v>
+      </c>
+      <c r="G246" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H246" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I246" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J246" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K246" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L246" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M246" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="N246" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O246" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P246" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q246" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R246" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S246" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T246" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U246" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V246" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W246" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X246" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y246" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z246" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA246" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB246" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC246" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD246" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="247" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A247" s="7">
+        <v>45569.82459074074</v>
+      </c>
+      <c r="B247" s="8" t="s">
+        <v>681</v>
+      </c>
+      <c r="C247" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D247" s="8">
+        <v>20227078</v>
+      </c>
+      <c r="E247" s="8" t="s">
+        <v>682</v>
+      </c>
+      <c r="F247" s="8">
+        <v>3</v>
+      </c>
+      <c r="G247" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H247" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I247" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J247" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K247" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L247" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M247" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N247" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O247" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P247" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q247" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R247" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S247" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T247" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U247" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V247" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W247" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X247" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y247" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z247" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA247" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB247" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC247" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD247" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="248" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A248" s="4">
+        <v>45569.828490659726</v>
+      </c>
+      <c r="B248" s="5" t="s">
+        <v>683</v>
+      </c>
+      <c r="C248" s="5" t="s">
+        <v>684</v>
+      </c>
+      <c r="D248" s="5">
+        <v>20205165</v>
+      </c>
+      <c r="E248" s="5" t="s">
+        <v>685</v>
+      </c>
+      <c r="F248" s="5">
+        <v>3</v>
+      </c>
+      <c r="G248" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H248" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I248" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J248" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K248" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L248" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M248" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N248" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O248" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P248" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q248" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R248" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S248" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T248" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U248" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V248" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W248" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X248" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y248" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z248" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA248" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB248" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC248" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD248" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="249" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A249" s="7">
+        <v>45569.839320231476</v>
+      </c>
+      <c r="B249" s="8" t="s">
+        <v>686</v>
+      </c>
+      <c r="C249" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D249" s="8">
+        <v>20192876</v>
+      </c>
+      <c r="E249" s="8" t="s">
+        <v>687</v>
+      </c>
+      <c r="F249" s="8">
+        <v>3</v>
+      </c>
+      <c r="G249" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H249" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I249" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J249" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K249" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L249" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M249" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N249" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O249" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P249" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q249" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R249" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S249" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T249" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U249" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V249" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W249" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X249" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y249" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z249" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA249" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB249" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC249" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD249" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="250" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A250" s="4">
+        <v>45569.860826018514</v>
+      </c>
+      <c r="B250" s="5" t="s">
+        <v>688</v>
+      </c>
+      <c r="C250" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="D250" s="5">
+        <v>20241515</v>
+      </c>
+      <c r="E250" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="F250" s="5">
+        <v>3</v>
+      </c>
+      <c r="G250" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="H250" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I250" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="J250" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="K250" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L250" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M250" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="N250" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O250" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P250" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q250" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="R250" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="S250" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="T250" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="U250" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V250" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W250" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="X250" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y250" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z250" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA250" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB250" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC250" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="AD250" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="251" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A251" s="7">
+        <v>45569.876496805555</v>
+      </c>
+      <c r="B251" s="8" t="s">
+        <v>689</v>
+      </c>
+      <c r="C251" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="D251" s="8">
+        <v>20182436</v>
+      </c>
+      <c r="E251" s="8" t="s">
+        <v>690</v>
+      </c>
+      <c r="F251" s="8">
+        <v>3</v>
+      </c>
+      <c r="G251" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H251" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I251" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J251" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K251" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L251" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M251" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N251" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O251" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P251" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q251" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R251" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S251" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T251" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U251" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V251" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W251" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X251" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y251" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z251" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA251" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB251" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC251" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD251" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="252" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A252" s="4">
+        <v>45569.893778634258</v>
+      </c>
+      <c r="B252" s="5" t="s">
+        <v>691</v>
+      </c>
+      <c r="C252" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="D252" s="5">
+        <v>20193305</v>
+      </c>
+      <c r="E252" s="5" t="s">
+        <v>692</v>
+      </c>
+      <c r="F252" s="5">
+        <v>3</v>
+      </c>
+      <c r="G252" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H252" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I252" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J252" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K252" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L252" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M252" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N252" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O252" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P252" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q252" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R252" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S252" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T252" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="U252" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V252" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W252" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X252" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y252" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z252" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA252" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB252" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC252" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD252" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="253" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A253" s="13">
+        <v>45569.901048414351</v>
+      </c>
+      <c r="B253" s="14" t="s">
+        <v>693</v>
+      </c>
+      <c r="C253" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D253" s="14">
+        <v>20242122</v>
+      </c>
+      <c r="E253" s="14" t="s">
+        <v>694</v>
+      </c>
+      <c r="F253" s="14">
+        <v>3</v>
+      </c>
+      <c r="G253" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H253" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="I253" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J253" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="K253" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="L253" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="M253" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N253" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="O253" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P253" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q253" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="R253" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="S253" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="T253" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="U253" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="V253" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="W253" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="X253" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y253" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z253" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA253" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB253" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC253" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD253" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
literacy, 240930 modified 7
</commit_message>
<xml_diff>
--- a/R/data/literacy_240930.xlsx
+++ b/R/data/literacy_240930.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC2A6E9-ED0F-244E-A46D-039A7155B195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B1DC13-6A44-2245-8572-701C5FE076BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50400" yWindow="1360" windowWidth="44800" windowHeight="24700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6834" uniqueCount="695">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7347" uniqueCount="735">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -2105,6 +2105,126 @@
   </si>
   <si>
     <t>손민재</t>
+  </si>
+  <si>
+    <t>yongwoo7701@gmail.com</t>
+  </si>
+  <si>
+    <t>유용우</t>
+  </si>
+  <si>
+    <t>rivernine369@naver.com</t>
+  </si>
+  <si>
+    <t>강재구</t>
+  </si>
+  <si>
+    <t>limjh3027@naver.com</t>
+  </si>
+  <si>
+    <t>임종현</t>
+  </si>
+  <si>
+    <t>nurasun050718@naver.com</t>
+  </si>
+  <si>
+    <t>이주연</t>
+  </si>
+  <si>
+    <t>kwakmin427@gmail.com</t>
+  </si>
+  <si>
+    <t>곽민규</t>
+  </si>
+  <si>
+    <t>kcwel1109@gmail.com</t>
+  </si>
+  <si>
+    <t>고미연</t>
+  </si>
+  <si>
+    <t>taewon16@naver.com</t>
+  </si>
+  <si>
+    <t>류태원</t>
+  </si>
+  <si>
+    <t>y5het3e@naver.com</t>
+  </si>
+  <si>
+    <t>박재근</t>
+  </si>
+  <si>
+    <t>a01053076907@gmail.com</t>
+  </si>
+  <si>
+    <t>원은성</t>
+  </si>
+  <si>
+    <t>lg01022928122@gmail.com</t>
+  </si>
+  <si>
+    <t>권주용</t>
+  </si>
+  <si>
+    <t>a35142191@gmail.com</t>
+  </si>
+  <si>
+    <t>이윤재</t>
+  </si>
+  <si>
+    <t>tngusvhs@gmail.com</t>
+  </si>
+  <si>
+    <t>이수현</t>
+  </si>
+  <si>
+    <t>wonda322@gmail.com</t>
+  </si>
+  <si>
+    <t>글로벌학부</t>
+  </si>
+  <si>
+    <t>원다연</t>
+  </si>
+  <si>
+    <t>ysh050116@naver.com</t>
+  </si>
+  <si>
+    <t>윤시한</t>
+  </si>
+  <si>
+    <t>shinsohee@naver.com</t>
+  </si>
+  <si>
+    <t>디지털미디어컨텐츠학과</t>
+  </si>
+  <si>
+    <t>신소희</t>
+  </si>
+  <si>
+    <t>cheun0423@gmail.com</t>
+  </si>
+  <si>
+    <t>이채은</t>
+  </si>
+  <si>
+    <t>ms071207@naver.com</t>
+  </si>
+  <si>
+    <t>sdw20050421@gmail.com</t>
+  </si>
+  <si>
+    <t>송도원</t>
+  </si>
+  <si>
+    <t>mt1661@naver.com</t>
+  </si>
+  <si>
+    <t>콘탠츠IT</t>
+  </si>
+  <si>
+    <t>정성민</t>
   </si>
 </sst>
 </file>
@@ -2519,7 +2639,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:AD253">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:AD272">
   <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -2757,11 +2877,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD253"/>
+  <dimension ref="A1:AD272"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E255" sqref="E255"/>
+      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C280" sqref="C280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -26070,6 +26190,1754 @@
         <v>56</v>
       </c>
     </row>
+    <row r="254" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A254" s="4">
+        <v>45569.911001157408</v>
+      </c>
+      <c r="B254" s="5" t="s">
+        <v>695</v>
+      </c>
+      <c r="C254" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D254" s="5">
+        <v>20244130</v>
+      </c>
+      <c r="E254" s="5" t="s">
+        <v>696</v>
+      </c>
+      <c r="F254" s="5">
+        <v>3</v>
+      </c>
+      <c r="G254" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H254" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I254" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J254" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K254" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L254" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M254" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N254" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O254" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P254" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q254" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R254" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S254" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T254" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U254" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="V254" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W254" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X254" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y254" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z254" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA254" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB254" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC254" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD254" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="255" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A255" s="7">
+        <v>45569.920861041668</v>
+      </c>
+      <c r="B255" s="8" t="s">
+        <v>697</v>
+      </c>
+      <c r="C255" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D255" s="8">
+        <v>20212801</v>
+      </c>
+      <c r="E255" s="8" t="s">
+        <v>698</v>
+      </c>
+      <c r="F255" s="8">
+        <v>3</v>
+      </c>
+      <c r="G255" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H255" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I255" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J255" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K255" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L255" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M255" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N255" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O255" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P255" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q255" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R255" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S255" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="T255" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U255" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V255" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W255" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X255" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y255" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z255" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA255" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB255" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC255" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD255" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="256" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A256" s="4">
+        <v>45569.922360474535</v>
+      </c>
+      <c r="B256" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="C256" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="D256" s="5">
+        <v>20242430</v>
+      </c>
+      <c r="E256" s="5" t="s">
+        <v>700</v>
+      </c>
+      <c r="F256" s="5">
+        <v>3</v>
+      </c>
+      <c r="G256" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H256" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I256" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J256" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K256" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L256" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M256" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="N256" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O256" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="P256" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q256" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="R256" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="S256" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="T256" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U256" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V256" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W256" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="X256" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="Y256" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z256" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA256" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB256" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC256" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD256" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="257" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A257" s="7">
+        <v>45569.943021087965</v>
+      </c>
+      <c r="B257" s="8" t="s">
+        <v>701</v>
+      </c>
+      <c r="C257" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="D257" s="8">
+        <v>20243636</v>
+      </c>
+      <c r="E257" s="8" t="s">
+        <v>702</v>
+      </c>
+      <c r="F257" s="8">
+        <v>3</v>
+      </c>
+      <c r="G257" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H257" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I257" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J257" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K257" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L257" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M257" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N257" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O257" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P257" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q257" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R257" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S257" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T257" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U257" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V257" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W257" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X257" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y257" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z257" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA257" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB257" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC257" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD257" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="258" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A258" s="4">
+        <v>45569.96052523148</v>
+      </c>
+      <c r="B258" s="5" t="s">
+        <v>703</v>
+      </c>
+      <c r="C258" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="D258" s="5">
+        <v>20243605</v>
+      </c>
+      <c r="E258" s="5" t="s">
+        <v>704</v>
+      </c>
+      <c r="F258" s="5">
+        <v>3</v>
+      </c>
+      <c r="G258" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H258" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I258" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J258" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K258" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L258" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M258" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N258" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O258" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P258" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q258" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R258" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S258" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T258" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="U258" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="V258" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W258" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="X258" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y258" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z258" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA258" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB258" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC258" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD258" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="259" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A259" s="7">
+        <v>45569.962306932866</v>
+      </c>
+      <c r="B259" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="C259" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D259" s="8">
+        <v>20246204</v>
+      </c>
+      <c r="E259" s="8" t="s">
+        <v>706</v>
+      </c>
+      <c r="F259" s="8">
+        <v>3</v>
+      </c>
+      <c r="G259" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H259" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I259" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J259" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K259" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="L259" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M259" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N259" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O259" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P259" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q259" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R259" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S259" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T259" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U259" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V259" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W259" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X259" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y259" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z259" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA259" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB259" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC259" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD259" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="260" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A260" s="4">
+        <v>45569.962533356476</v>
+      </c>
+      <c r="B260" s="5" t="s">
+        <v>707</v>
+      </c>
+      <c r="C260" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="D260" s="5">
+        <v>20195158</v>
+      </c>
+      <c r="E260" s="5" t="s">
+        <v>708</v>
+      </c>
+      <c r="F260" s="5">
+        <v>3</v>
+      </c>
+      <c r="G260" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H260" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I260" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J260" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="K260" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L260" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M260" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="N260" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O260" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P260" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q260" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R260" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S260" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T260" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U260" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V260" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W260" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X260" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y260" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z260" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA260" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB260" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC260" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD260" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="261" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A261" s="7">
+        <v>45569.971057222225</v>
+      </c>
+      <c r="B261" s="8" t="s">
+        <v>709</v>
+      </c>
+      <c r="C261" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D261" s="8">
+        <v>20215158</v>
+      </c>
+      <c r="E261" s="8" t="s">
+        <v>710</v>
+      </c>
+      <c r="F261" s="8">
+        <v>3</v>
+      </c>
+      <c r="G261" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H261" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I261" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J261" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="K261" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L261" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M261" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N261" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O261" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P261" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q261" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R261" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S261" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T261" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U261" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V261" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="W261" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X261" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y261" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z261" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA261" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB261" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC261" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD261" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="262" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A262" s="4">
+        <v>45569.984572349538</v>
+      </c>
+      <c r="B262" s="5" t="s">
+        <v>711</v>
+      </c>
+      <c r="C262" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="D262" s="5">
+        <v>20246927</v>
+      </c>
+      <c r="E262" s="5" t="s">
+        <v>712</v>
+      </c>
+      <c r="F262" s="5">
+        <v>3</v>
+      </c>
+      <c r="G262" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H262" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I262" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J262" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K262" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L262" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M262" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N262" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O262" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P262" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q262" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R262" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S262" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T262" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U262" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V262" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W262" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X262" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y262" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z262" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA262" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB262" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC262" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD262" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="263" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A263" s="7">
+        <v>45569.991886909724</v>
+      </c>
+      <c r="B263" s="8" t="s">
+        <v>713</v>
+      </c>
+      <c r="C263" s="8" t="s">
+        <v>485</v>
+      </c>
+      <c r="D263" s="8">
+        <v>20215109</v>
+      </c>
+      <c r="E263" s="8" t="s">
+        <v>714</v>
+      </c>
+      <c r="F263" s="8">
+        <v>3</v>
+      </c>
+      <c r="G263" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H263" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I263" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J263" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K263" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="L263" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M263" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N263" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O263" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P263" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q263" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R263" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S263" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T263" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="U263" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V263" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W263" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X263" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y263" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z263" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA263" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB263" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC263" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD263" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="264" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A264" s="4">
+        <v>45570.039893113426</v>
+      </c>
+      <c r="B264" s="5" t="s">
+        <v>715</v>
+      </c>
+      <c r="C264" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D264" s="5">
+        <v>20243241</v>
+      </c>
+      <c r="E264" s="5" t="s">
+        <v>716</v>
+      </c>
+      <c r="F264" s="5">
+        <v>3</v>
+      </c>
+      <c r="G264" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H264" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I264" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J264" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K264" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="L264" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M264" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N264" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O264" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P264" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q264" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R264" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S264" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T264" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U264" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V264" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W264" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X264" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y264" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z264" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA264" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB264" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC264" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD264" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="265" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A265" s="7">
+        <v>45570.04225569444</v>
+      </c>
+      <c r="B265" s="8" t="s">
+        <v>717</v>
+      </c>
+      <c r="C265" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="D265" s="8">
+        <v>20243529</v>
+      </c>
+      <c r="E265" s="8" t="s">
+        <v>718</v>
+      </c>
+      <c r="F265" s="8">
+        <v>3</v>
+      </c>
+      <c r="G265" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H265" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I265" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J265" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K265" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L265" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M265" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N265" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O265" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P265" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q265" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R265" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S265" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T265" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U265" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V265" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W265" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X265" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y265" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z265" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA265" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB265" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC265" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD265" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="266" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A266" s="4">
+        <v>45570.049677106479</v>
+      </c>
+      <c r="B266" s="5" t="s">
+        <v>719</v>
+      </c>
+      <c r="C266" s="5" t="s">
+        <v>720</v>
+      </c>
+      <c r="D266" s="5">
+        <v>20246414</v>
+      </c>
+      <c r="E266" s="5" t="s">
+        <v>721</v>
+      </c>
+      <c r="F266" s="5">
+        <v>3</v>
+      </c>
+      <c r="G266" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H266" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I266" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J266" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K266" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L266" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M266" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N266" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O266" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P266" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q266" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R266" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S266" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T266" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U266" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V266" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W266" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X266" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y266" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z266" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA266" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB266" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC266" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD266" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="267" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A267" s="7">
+        <v>45570.07502275463</v>
+      </c>
+      <c r="B267" s="8" t="s">
+        <v>722</v>
+      </c>
+      <c r="C267" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="D267" s="8">
+        <v>20246752</v>
+      </c>
+      <c r="E267" s="8" t="s">
+        <v>723</v>
+      </c>
+      <c r="F267" s="8">
+        <v>3</v>
+      </c>
+      <c r="G267" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="H267" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I267" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="J267" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="K267" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="L267" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M267" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N267" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O267" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="P267" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q267" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R267" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="S267" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="T267" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U267" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="V267" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W267" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X267" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y267" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z267" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA267" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB267" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC267" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD267" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="268" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A268" s="4">
+        <v>45570.093391898146</v>
+      </c>
+      <c r="B268" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="C268" s="5" t="s">
+        <v>725</v>
+      </c>
+      <c r="D268" s="5">
+        <v>20235198</v>
+      </c>
+      <c r="E268" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="F268" s="5">
+        <v>3</v>
+      </c>
+      <c r="G268" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H268" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I268" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J268" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="K268" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L268" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M268" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N268" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O268" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P268" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q268" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R268" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S268" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T268" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U268" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="V268" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W268" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X268" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y268" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z268" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA268" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB268" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC268" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD268" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="269" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A269" s="7">
+        <v>45570.105374317129</v>
+      </c>
+      <c r="B269" s="8" t="s">
+        <v>727</v>
+      </c>
+      <c r="C269" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D269" s="8">
+        <v>20217152</v>
+      </c>
+      <c r="E269" s="8" t="s">
+        <v>728</v>
+      </c>
+      <c r="F269" s="8">
+        <v>3</v>
+      </c>
+      <c r="G269" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H269" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I269" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J269" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K269" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L269" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M269" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N269" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O269" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P269" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q269" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R269" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S269" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T269" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U269" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V269" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W269" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X269" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y269" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z269" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA269" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB269" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC269" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD269" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="270" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A270" s="16">
+        <v>45570.1759652662</v>
+      </c>
+      <c r="B270" s="17" t="s">
+        <v>729</v>
+      </c>
+      <c r="C270" s="17" t="s">
+        <v>324</v>
+      </c>
+      <c r="D270" s="17">
+        <v>20193644</v>
+      </c>
+      <c r="E270" s="17" t="s">
+        <v>530</v>
+      </c>
+      <c r="F270" s="17">
+        <v>3</v>
+      </c>
+      <c r="G270" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H270" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="I270" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="J270" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="K270" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="L270" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="M270" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="N270" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="O270" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="P270" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q270" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="R270" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="S270" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="T270" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="U270" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="V270" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="W270" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="X270" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y270" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z270" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA270" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB270" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC270" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD270" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="271" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A271" s="7">
+        <v>45570.383973530093</v>
+      </c>
+      <c r="B271" s="8" t="s">
+        <v>730</v>
+      </c>
+      <c r="C271" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="D271" s="8">
+        <v>20242418</v>
+      </c>
+      <c r="E271" s="8" t="s">
+        <v>731</v>
+      </c>
+      <c r="F271" s="8">
+        <v>3</v>
+      </c>
+      <c r="G271" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H271" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I271" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J271" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K271" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L271" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M271" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N271" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O271" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P271" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q271" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R271" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S271" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T271" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U271" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V271" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W271" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X271" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y271" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z271" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA271" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB271" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC271" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD271" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="272" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A272" s="16">
+        <v>45570.444734363424</v>
+      </c>
+      <c r="B272" s="17" t="s">
+        <v>732</v>
+      </c>
+      <c r="C272" s="17" t="s">
+        <v>733</v>
+      </c>
+      <c r="D272" s="17">
+        <v>20215239</v>
+      </c>
+      <c r="E272" s="17" t="s">
+        <v>734</v>
+      </c>
+      <c r="F272" s="17">
+        <v>3</v>
+      </c>
+      <c r="G272" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H272" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="I272" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="J272" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="K272" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="L272" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="M272" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="N272" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="O272" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="P272" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q272" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="R272" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="S272" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="T272" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="U272" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="V272" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="W272" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="X272" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="Y272" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z272" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="AA272" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB272" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC272" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="AD272" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
literacy, 240930 modified 8
</commit_message>
<xml_diff>
--- a/R/data/literacy_240930.xlsx
+++ b/R/data/literacy_240930.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B1DC13-6A44-2245-8572-701C5FE076BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD443E1-D5FB-F34E-9FF9-822F20E30E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50400" yWindow="1360" windowWidth="44800" windowHeight="24700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7347" uniqueCount="735">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8103" uniqueCount="794">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -2225,6 +2225,183 @@
   </si>
   <si>
     <t>정성민</t>
+  </si>
+  <si>
+    <t>stacy4036@naver.com</t>
+  </si>
+  <si>
+    <t>최하은</t>
+  </si>
+  <si>
+    <t>tjtkdwns0909@naver.com</t>
+  </si>
+  <si>
+    <t>서상준</t>
+  </si>
+  <si>
+    <t>thwls5541@gmail.com</t>
+  </si>
+  <si>
+    <t>김소원</t>
+  </si>
+  <si>
+    <t>kyj57980@gmail.com</t>
+  </si>
+  <si>
+    <t>김예진</t>
+  </si>
+  <si>
+    <t>dohan5453@gmail.com</t>
+  </si>
+  <si>
+    <t>김도한</t>
+  </si>
+  <si>
+    <t>ryul1128@naver.com</t>
+  </si>
+  <si>
+    <t>김률아</t>
+  </si>
+  <si>
+    <t>ahrang1225@gmail.com</t>
+  </si>
+  <si>
+    <t>탁아랑</t>
+  </si>
+  <si>
+    <t>oys55736@gmail.com</t>
+  </si>
+  <si>
+    <t>오윤서</t>
+  </si>
+  <si>
+    <t>123plokml123@gmail.com</t>
+  </si>
+  <si>
+    <t>지현배</t>
+  </si>
+  <si>
+    <t>leeyubin050328@naver.com</t>
+  </si>
+  <si>
+    <t>jin050828@gmail.com</t>
+  </si>
+  <si>
+    <t>김진영</t>
+  </si>
+  <si>
+    <t>kbi70722@gmail.com</t>
+  </si>
+  <si>
+    <t>김병일</t>
+  </si>
+  <si>
+    <t>quddus6378@gmail.com</t>
+  </si>
+  <si>
+    <t>현병연</t>
+  </si>
+  <si>
+    <t>1. 권찬기 씨와 김서경 씨가 결혼한다.</t>
+  </si>
+  <si>
+    <t>wlsqhwlsqh21@naver.com</t>
+  </si>
+  <si>
+    <t>경영학부</t>
+  </si>
+  <si>
+    <t>심진보</t>
+  </si>
+  <si>
+    <t>0524psu@gmail.com</t>
+  </si>
+  <si>
+    <t>박상언</t>
+  </si>
+  <si>
+    <t>ella2005710@gmail.com</t>
+  </si>
+  <si>
+    <t>김송이</t>
+  </si>
+  <si>
+    <t>dbfrhr02@naver.com</t>
+  </si>
+  <si>
+    <t>심건휘</t>
+  </si>
+  <si>
+    <t>1kdcf@naver.com</t>
+  </si>
+  <si>
+    <t>송준영</t>
+  </si>
+  <si>
+    <t>hm703711@gmail.com</t>
+  </si>
+  <si>
+    <t>언론방송융합미디어학과</t>
+  </si>
+  <si>
+    <t>박현민</t>
+  </si>
+  <si>
+    <t>gangjunu@naver.com</t>
+  </si>
+  <si>
+    <t>강준우</t>
+  </si>
+  <si>
+    <t>xodet0817@naver.com</t>
+  </si>
+  <si>
+    <t>문종윤</t>
+  </si>
+  <si>
+    <t>benjamin27@naver.com</t>
+  </si>
+  <si>
+    <t>디지털미디어학부</t>
+  </si>
+  <si>
+    <t>최재혁</t>
+  </si>
+  <si>
+    <t>towp7563@gmail.com</t>
+  </si>
+  <si>
+    <t>오승현</t>
+  </si>
+  <si>
+    <t>seoeunchan5@gmail.com</t>
+  </si>
+  <si>
+    <t>서은찬</t>
+  </si>
+  <si>
+    <t>eojeongmin146@gmail.com</t>
+  </si>
+  <si>
+    <t>어정민</t>
+  </si>
+  <si>
+    <t>rer220@naver.com</t>
+  </si>
+  <si>
+    <t>김대명</t>
+  </si>
+  <si>
+    <t>jyb051128@gmail.com</t>
+  </si>
+  <si>
+    <t>전유빈</t>
+  </si>
+  <si>
+    <t>gmlfkr6241@naver.com</t>
+  </si>
+  <si>
+    <t>한희락</t>
   </si>
 </sst>
 </file>
@@ -2639,7 +2816,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:AD272">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:AD300">
   <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -2877,11 +3054,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD272"/>
+  <dimension ref="A1:AD300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C280" sqref="C280"/>
+      <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D321" sqref="D321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -27938,6 +28115,2582 @@
         <v>56</v>
       </c>
     </row>
+    <row r="273" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A273" s="7">
+        <v>45570.492994918983</v>
+      </c>
+      <c r="B273" s="8" t="s">
+        <v>735</v>
+      </c>
+      <c r="C273" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="D273" s="8">
+        <v>20227034</v>
+      </c>
+      <c r="E273" s="8" t="s">
+        <v>736</v>
+      </c>
+      <c r="F273" s="8">
+        <v>3</v>
+      </c>
+      <c r="G273" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H273" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I273" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="J273" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="K273" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="L273" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="M273" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N273" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O273" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="P273" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q273" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="R273" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S273" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="T273" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U273" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V273" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="W273" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="X273" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="Y273" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z273" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA273" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB273" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC273" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD273" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="274" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A274" s="4">
+        <v>45570.497735879631</v>
+      </c>
+      <c r="B274" s="5" t="s">
+        <v>737</v>
+      </c>
+      <c r="C274" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D274" s="5">
+        <v>20244123</v>
+      </c>
+      <c r="E274" s="5" t="s">
+        <v>738</v>
+      </c>
+      <c r="F274" s="5">
+        <v>3</v>
+      </c>
+      <c r="G274" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H274" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I274" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J274" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K274" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L274" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M274" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N274" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O274" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P274" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q274" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R274" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S274" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T274" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="U274" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V274" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W274" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X274" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y274" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z274" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA274" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB274" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC274" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD274" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="275" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A275" s="7">
+        <v>45570.516114062499</v>
+      </c>
+      <c r="B275" s="8" t="s">
+        <v>739</v>
+      </c>
+      <c r="C275" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D275" s="8">
+        <v>20207065</v>
+      </c>
+      <c r="E275" s="8" t="s">
+        <v>740</v>
+      </c>
+      <c r="F275" s="8">
+        <v>3</v>
+      </c>
+      <c r="G275" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H275" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I275" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J275" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K275" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L275" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M275" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N275" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O275" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P275" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q275" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R275" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S275" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T275" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U275" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V275" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="W275" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X275" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y275" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z275" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA275" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB275" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC275" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD275" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="276" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A276" s="4">
+        <v>45570.54779759259</v>
+      </c>
+      <c r="B276" s="5" t="s">
+        <v>741</v>
+      </c>
+      <c r="C276" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="D276" s="5">
+        <v>20202319</v>
+      </c>
+      <c r="E276" s="5" t="s">
+        <v>742</v>
+      </c>
+      <c r="F276" s="5">
+        <v>3</v>
+      </c>
+      <c r="G276" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H276" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I276" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J276" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K276" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L276" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M276" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N276" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O276" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P276" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q276" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R276" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S276" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T276" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U276" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V276" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W276" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X276" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y276" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z276" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA276" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB276" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC276" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD276" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="277" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A277" s="7">
+        <v>45570.564522581015</v>
+      </c>
+      <c r="B277" s="8" t="s">
+        <v>743</v>
+      </c>
+      <c r="C277" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D277" s="8">
+        <v>20225117</v>
+      </c>
+      <c r="E277" s="8" t="s">
+        <v>744</v>
+      </c>
+      <c r="F277" s="8">
+        <v>3</v>
+      </c>
+      <c r="G277" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H277" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I277" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J277" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K277" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L277" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M277" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N277" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O277" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="P277" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q277" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="R277" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="S277" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="T277" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U277" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V277" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W277" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="X277" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y277" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z277" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA277" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB277" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC277" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD277" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="278" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A278" s="4">
+        <v>45570.565115104167</v>
+      </c>
+      <c r="B278" s="5" t="s">
+        <v>745</v>
+      </c>
+      <c r="C278" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D278" s="5">
+        <v>20243806</v>
+      </c>
+      <c r="E278" s="5" t="s">
+        <v>746</v>
+      </c>
+      <c r="F278" s="5">
+        <v>3</v>
+      </c>
+      <c r="G278" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H278" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I278" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J278" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K278" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L278" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M278" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N278" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O278" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P278" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q278" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R278" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S278" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T278" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U278" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V278" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W278" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X278" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y278" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z278" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA278" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB278" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC278" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD278" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="279" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A279" s="7">
+        <v>45570.567347534721</v>
+      </c>
+      <c r="B279" s="8" t="s">
+        <v>747</v>
+      </c>
+      <c r="C279" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="D279" s="8">
+        <v>20242240</v>
+      </c>
+      <c r="E279" s="8" t="s">
+        <v>748</v>
+      </c>
+      <c r="F279" s="8">
+        <v>3</v>
+      </c>
+      <c r="G279" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H279" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I279" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J279" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="K279" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="L279" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M279" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N279" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O279" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="P279" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q279" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R279" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S279" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T279" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U279" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V279" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W279" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X279" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y279" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z279" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA279" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB279" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC279" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD279" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="280" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A280" s="4">
+        <v>45570.569745601853</v>
+      </c>
+      <c r="B280" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="C280" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D280" s="5">
+        <v>20242332</v>
+      </c>
+      <c r="E280" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="F280" s="5">
+        <v>3</v>
+      </c>
+      <c r="G280" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H280" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I280" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J280" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="K280" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="L280" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M280" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N280" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O280" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P280" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q280" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R280" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S280" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="T280" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U280" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V280" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="W280" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X280" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y280" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z280" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA280" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB280" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC280" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD280" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="281" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A281" s="7">
+        <v>45570.580681157408</v>
+      </c>
+      <c r="B281" s="8" t="s">
+        <v>751</v>
+      </c>
+      <c r="C281" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D281" s="8">
+        <v>20245266</v>
+      </c>
+      <c r="E281" s="8" t="s">
+        <v>752</v>
+      </c>
+      <c r="F281" s="8">
+        <v>1</v>
+      </c>
+      <c r="G281" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="H281" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I281" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J281" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K281" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L281" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="M281" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N281" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O281" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="P281" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q281" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="R281" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S281" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T281" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U281" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V281" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W281" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="X281" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y281" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z281" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA281" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB281" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC281" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD281" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="282" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A282" s="4">
+        <v>45570.589595590282</v>
+      </c>
+      <c r="B282" s="5" t="s">
+        <v>753</v>
+      </c>
+      <c r="C282" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="D282" s="5">
+        <v>20243008</v>
+      </c>
+      <c r="E282" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="F282" s="5">
+        <v>3</v>
+      </c>
+      <c r="G282" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H282" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I282" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J282" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K282" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L282" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M282" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N282" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O282" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P282" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q282" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R282" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S282" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T282" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U282" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V282" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W282" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X282" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y282" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z282" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA282" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB282" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC282" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD282" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="283" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A283" s="7">
+        <v>45570.61784600695</v>
+      </c>
+      <c r="B283" s="8" t="s">
+        <v>754</v>
+      </c>
+      <c r="C283" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="D283" s="8">
+        <v>20246715</v>
+      </c>
+      <c r="E283" s="8" t="s">
+        <v>755</v>
+      </c>
+      <c r="F283" s="8">
+        <v>3</v>
+      </c>
+      <c r="G283" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H283" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I283" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J283" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K283" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L283" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M283" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N283" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O283" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P283" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q283" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R283" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="S283" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T283" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U283" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V283" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W283" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X283" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y283" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z283" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA283" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB283" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC283" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD283" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="284" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A284" s="4">
+        <v>45570.639197731478</v>
+      </c>
+      <c r="B284" s="5" t="s">
+        <v>756</v>
+      </c>
+      <c r="C284" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D284" s="5">
+        <v>20191604</v>
+      </c>
+      <c r="E284" s="5" t="s">
+        <v>757</v>
+      </c>
+      <c r="F284" s="5">
+        <v>3</v>
+      </c>
+      <c r="G284" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H284" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I284" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J284" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K284" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L284" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M284" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N284" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O284" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P284" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q284" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R284" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S284" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T284" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U284" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V284" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W284" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X284" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y284" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z284" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA284" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB284" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC284" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD284" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="285" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A285" s="7">
+        <v>45570.639488981484</v>
+      </c>
+      <c r="B285" s="8" t="s">
+        <v>758</v>
+      </c>
+      <c r="C285" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D285" s="8">
+        <v>20227106</v>
+      </c>
+      <c r="E285" s="8" t="s">
+        <v>759</v>
+      </c>
+      <c r="F285" s="8">
+        <v>3</v>
+      </c>
+      <c r="G285" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="H285" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I285" s="8" t="s">
+        <v>760</v>
+      </c>
+      <c r="J285" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="K285" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L285" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="M285" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N285" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O285" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="P285" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q285" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R285" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="S285" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="T285" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U285" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="V285" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="W285" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="X285" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y285" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z285" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="AA285" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB285" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC285" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="AD285" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="286" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A286" s="4">
+        <v>45570.654147118054</v>
+      </c>
+      <c r="B286" s="5" t="s">
+        <v>761</v>
+      </c>
+      <c r="C286" s="5" t="s">
+        <v>762</v>
+      </c>
+      <c r="D286" s="5">
+        <v>20242982</v>
+      </c>
+      <c r="E286" s="5" t="s">
+        <v>763</v>
+      </c>
+      <c r="F286" s="5">
+        <v>3</v>
+      </c>
+      <c r="G286" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H286" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I286" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J286" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K286" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L286" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M286" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N286" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O286" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P286" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q286" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R286" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S286" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T286" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U286" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V286" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W286" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X286" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y286" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z286" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA286" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB286" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC286" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD286" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="287" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A287" s="7">
+        <v>45570.66921472222</v>
+      </c>
+      <c r="B287" s="8" t="s">
+        <v>764</v>
+      </c>
+      <c r="C287" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D287" s="8">
+        <v>20243713</v>
+      </c>
+      <c r="E287" s="8" t="s">
+        <v>765</v>
+      </c>
+      <c r="F287" s="8">
+        <v>3</v>
+      </c>
+      <c r="G287" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H287" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I287" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J287" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K287" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L287" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M287" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N287" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O287" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P287" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q287" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R287" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S287" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T287" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="U287" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V287" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W287" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X287" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y287" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z287" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA287" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB287" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC287" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD287" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="288" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A288" s="4">
+        <v>45570.674444537042</v>
+      </c>
+      <c r="B288" s="5" t="s">
+        <v>766</v>
+      </c>
+      <c r="C288" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D288" s="5">
+        <v>20246222</v>
+      </c>
+      <c r="E288" s="5" t="s">
+        <v>767</v>
+      </c>
+      <c r="F288" s="5">
+        <v>3</v>
+      </c>
+      <c r="G288" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H288" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I288" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J288" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K288" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="L288" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M288" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N288" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O288" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P288" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q288" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R288" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S288" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T288" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U288" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V288" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W288" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X288" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y288" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z288" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA288" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB288" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC288" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD288" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="289" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A289" s="7">
+        <v>45570.675514409726</v>
+      </c>
+      <c r="B289" s="8" t="s">
+        <v>768</v>
+      </c>
+      <c r="C289" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D289" s="8">
+        <v>20212971</v>
+      </c>
+      <c r="E289" s="8" t="s">
+        <v>769</v>
+      </c>
+      <c r="F289" s="8">
+        <v>3</v>
+      </c>
+      <c r="G289" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H289" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I289" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J289" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K289" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="L289" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M289" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="N289" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O289" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P289" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q289" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R289" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S289" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T289" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U289" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V289" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W289" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X289" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y289" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z289" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA289" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB289" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC289" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD289" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="290" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A290" s="4">
+        <v>45570.685494363424</v>
+      </c>
+      <c r="B290" s="5" t="s">
+        <v>770</v>
+      </c>
+      <c r="C290" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D290" s="5">
+        <v>20192901</v>
+      </c>
+      <c r="E290" s="5" t="s">
+        <v>771</v>
+      </c>
+      <c r="F290" s="5">
+        <v>3</v>
+      </c>
+      <c r="G290" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H290" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I290" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J290" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K290" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L290" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M290" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N290" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O290" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P290" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q290" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R290" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S290" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T290" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U290" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V290" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W290" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X290" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y290" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z290" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA290" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB290" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC290" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD290" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="291" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A291" s="7">
+        <v>45570.695558449079</v>
+      </c>
+      <c r="B291" s="8" t="s">
+        <v>772</v>
+      </c>
+      <c r="C291" s="8" t="s">
+        <v>773</v>
+      </c>
+      <c r="D291" s="8">
+        <v>20202415</v>
+      </c>
+      <c r="E291" s="8" t="s">
+        <v>774</v>
+      </c>
+      <c r="F291" s="8">
+        <v>3</v>
+      </c>
+      <c r="G291" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H291" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I291" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J291" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K291" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L291" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M291" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N291" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O291" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P291" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q291" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R291" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S291" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T291" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="U291" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V291" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W291" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X291" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y291" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z291" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA291" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB291" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC291" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD291" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="292" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A292" s="4">
+        <v>45570.696724583337</v>
+      </c>
+      <c r="B292" s="5" t="s">
+        <v>775</v>
+      </c>
+      <c r="C292" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D292" s="5">
+        <v>20242901</v>
+      </c>
+      <c r="E292" s="5" t="s">
+        <v>776</v>
+      </c>
+      <c r="F292" s="5">
+        <v>3</v>
+      </c>
+      <c r="G292" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H292" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I292" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J292" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K292" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L292" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M292" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N292" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O292" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P292" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q292" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R292" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S292" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T292" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U292" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V292" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W292" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X292" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y292" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z292" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA292" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB292" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC292" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD292" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="293" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A293" s="7">
+        <v>45570.700904375</v>
+      </c>
+      <c r="B293" s="8" t="s">
+        <v>777</v>
+      </c>
+      <c r="C293" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="D293" s="8">
+        <v>20203616</v>
+      </c>
+      <c r="E293" s="8" t="s">
+        <v>778</v>
+      </c>
+      <c r="F293" s="8">
+        <v>3</v>
+      </c>
+      <c r="G293" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H293" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I293" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J293" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K293" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L293" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M293" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N293" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O293" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P293" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q293" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R293" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S293" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T293" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U293" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V293" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W293" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X293" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y293" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z293" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA293" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB293" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC293" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD293" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="294" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A294" s="4">
+        <v>45570.704123645832</v>
+      </c>
+      <c r="B294" s="5" t="s">
+        <v>779</v>
+      </c>
+      <c r="C294" s="5" t="s">
+        <v>780</v>
+      </c>
+      <c r="D294" s="5">
+        <v>20212583</v>
+      </c>
+      <c r="E294" s="5" t="s">
+        <v>781</v>
+      </c>
+      <c r="F294" s="5">
+        <v>3</v>
+      </c>
+      <c r="G294" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H294" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I294" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J294" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K294" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L294" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M294" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N294" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O294" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P294" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q294" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R294" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S294" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T294" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U294" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V294" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W294" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X294" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y294" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z294" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA294" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB294" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC294" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD294" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="295" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A295" s="7">
+        <v>45570.704930219908</v>
+      </c>
+      <c r="B295" s="8" t="s">
+        <v>782</v>
+      </c>
+      <c r="C295" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D295" s="8">
+        <v>20243826</v>
+      </c>
+      <c r="E295" s="8" t="s">
+        <v>783</v>
+      </c>
+      <c r="F295" s="8">
+        <v>3</v>
+      </c>
+      <c r="G295" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H295" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I295" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J295" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K295" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L295" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M295" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N295" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O295" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P295" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q295" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R295" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="S295" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T295" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="U295" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V295" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="W295" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X295" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y295" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z295" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA295" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB295" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC295" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD295" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="296" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A296" s="4">
+        <v>45570.710447384263</v>
+      </c>
+      <c r="B296" s="5" t="s">
+        <v>784</v>
+      </c>
+      <c r="C296" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D296" s="5">
+        <v>20245183</v>
+      </c>
+      <c r="E296" s="5" t="s">
+        <v>785</v>
+      </c>
+      <c r="F296" s="5">
+        <v>3</v>
+      </c>
+      <c r="G296" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H296" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I296" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J296" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="K296" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L296" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M296" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="N296" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O296" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P296" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q296" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R296" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S296" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T296" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U296" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V296" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W296" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X296" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y296" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z296" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA296" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB296" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC296" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD296" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="297" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A297" s="7">
+        <v>45570.719198761573</v>
+      </c>
+      <c r="B297" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="C297" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D297" s="8">
+        <v>20242725</v>
+      </c>
+      <c r="E297" s="8" t="s">
+        <v>787</v>
+      </c>
+      <c r="F297" s="8">
+        <v>3</v>
+      </c>
+      <c r="G297" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H297" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I297" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J297" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K297" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="L297" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M297" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N297" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O297" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P297" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q297" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R297" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S297" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T297" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U297" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V297" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W297" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X297" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y297" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z297" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA297" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB297" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC297" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD297" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="298" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A298" s="4">
+        <v>45570.720825682874</v>
+      </c>
+      <c r="B298" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="C298" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D298" s="5">
+        <v>20205124</v>
+      </c>
+      <c r="E298" s="5" t="s">
+        <v>789</v>
+      </c>
+      <c r="F298" s="5">
+        <v>3</v>
+      </c>
+      <c r="G298" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H298" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I298" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J298" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K298" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L298" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M298" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N298" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O298" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="P298" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q298" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R298" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S298" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T298" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U298" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V298" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W298" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X298" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y298" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z298" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA298" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB298" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC298" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD298" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="299" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A299" s="7">
+        <v>45570.724715532408</v>
+      </c>
+      <c r="B299" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="C299" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="D299" s="8">
+        <v>20243646</v>
+      </c>
+      <c r="E299" s="8" t="s">
+        <v>791</v>
+      </c>
+      <c r="F299" s="8">
+        <v>3</v>
+      </c>
+      <c r="G299" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H299" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I299" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J299" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K299" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L299" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M299" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N299" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O299" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P299" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q299" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R299" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S299" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T299" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="U299" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="V299" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W299" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X299" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="Y299" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z299" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA299" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB299" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC299" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD299" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="300" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A300" s="16">
+        <v>45570.734741168984</v>
+      </c>
+      <c r="B300" s="17" t="s">
+        <v>792</v>
+      </c>
+      <c r="C300" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D300" s="17">
+        <v>20246303</v>
+      </c>
+      <c r="E300" s="17" t="s">
+        <v>793</v>
+      </c>
+      <c r="F300" s="17">
+        <v>3</v>
+      </c>
+      <c r="G300" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="H300" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="I300" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="J300" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="K300" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="L300" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="M300" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="N300" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="O300" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="P300" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q300" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="R300" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="S300" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="T300" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="U300" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="V300" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="W300" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="X300" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y300" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z300" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA300" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB300" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC300" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD300" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
literacy, 240930 modified 9
</commit_message>
<xml_diff>
--- a/R/data/literacy_240930.xlsx
+++ b/R/data/literacy_240930.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD443E1-D5FB-F34E-9FF9-822F20E30E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AD7725-A9D2-D64E-90F6-748C6282BC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50400" yWindow="1360" windowWidth="44800" windowHeight="24700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8103" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9183" uniqueCount="874">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -2402,6 +2402,246 @@
   </si>
   <si>
     <t>한희락</t>
+  </si>
+  <si>
+    <t>wweufc0913123456@gmail.com</t>
+  </si>
+  <si>
+    <t>지강민</t>
+  </si>
+  <si>
+    <t>kentoku0901@naver.com</t>
+  </si>
+  <si>
+    <t>김헌덕</t>
+  </si>
+  <si>
+    <t>andy9925@naver.com</t>
+  </si>
+  <si>
+    <t>김무극</t>
+  </si>
+  <si>
+    <t>junwoni20@gmail.com</t>
+  </si>
+  <si>
+    <t>이준원</t>
+  </si>
+  <si>
+    <t>to_csm@naver.com</t>
+  </si>
+  <si>
+    <t>천상미</t>
+  </si>
+  <si>
+    <t>tigerhaha1@naver.com</t>
+  </si>
+  <si>
+    <t>김민호</t>
+  </si>
+  <si>
+    <t>obokboki@naver.com</t>
+  </si>
+  <si>
+    <t>최서윤</t>
+  </si>
+  <si>
+    <t>ssjm9652@naver.com</t>
+  </si>
+  <si>
+    <t>소정민</t>
+  </si>
+  <si>
+    <t>iaan0104@naver.com</t>
+  </si>
+  <si>
+    <t>조이안</t>
+  </si>
+  <si>
+    <t>smarthulk0318@naver.com</t>
+  </si>
+  <si>
+    <t>조성민</t>
+  </si>
+  <si>
+    <t>ystop061012@naver.com</t>
+  </si>
+  <si>
+    <t>손연수</t>
+  </si>
+  <si>
+    <t>johyeram@gmail.com</t>
+  </si>
+  <si>
+    <t>조혜람</t>
+  </si>
+  <si>
+    <t>knh6654@gmail.com</t>
+  </si>
+  <si>
+    <t>김나현</t>
+  </si>
+  <si>
+    <t>Psj050317@naver.com</t>
+  </si>
+  <si>
+    <t>박서진</t>
+  </si>
+  <si>
+    <t>pdh9467472@gmail.com</t>
+  </si>
+  <si>
+    <t>박두환</t>
+  </si>
+  <si>
+    <t>raon2812@naver.com</t>
+  </si>
+  <si>
+    <t>최라온</t>
+  </si>
+  <si>
+    <t>inheo0428@gmail.com</t>
+  </si>
+  <si>
+    <t>허인</t>
+  </si>
+  <si>
+    <t>cmin0945@gmail.com</t>
+  </si>
+  <si>
+    <t>조상민</t>
+  </si>
+  <si>
+    <t>whovian2@naver.com</t>
+  </si>
+  <si>
+    <t>이새한</t>
+  </si>
+  <si>
+    <t>awinni@naver.com</t>
+  </si>
+  <si>
+    <t>우현진</t>
+  </si>
+  <si>
+    <t>mi88368836@gmail.com</t>
+  </si>
+  <si>
+    <t>신민서</t>
+  </si>
+  <si>
+    <t>kayla1071702@gmail.com</t>
+  </si>
+  <si>
+    <t>임혜빈</t>
+  </si>
+  <si>
+    <t>hhr0408@naver.com</t>
+  </si>
+  <si>
+    <t>한혜령</t>
+  </si>
+  <si>
+    <t>ab47cd32@gmail.com</t>
+  </si>
+  <si>
+    <t>우로겸</t>
+  </si>
+  <si>
+    <t>20242925@hallym.ac.kr</t>
+  </si>
+  <si>
+    <t>김민우</t>
+  </si>
+  <si>
+    <t>ann12ann1209@gmail.com</t>
+  </si>
+  <si>
+    <t>김혜원</t>
+  </si>
+  <si>
+    <t>nyo07@naver.com</t>
+  </si>
+  <si>
+    <t>윤효라</t>
+  </si>
+  <si>
+    <t>youngold057@gmail.com</t>
+  </si>
+  <si>
+    <t>윤태영</t>
+  </si>
+  <si>
+    <t>corki1234@naver.com</t>
+  </si>
+  <si>
+    <t>윤서웅</t>
+  </si>
+  <si>
+    <t>ujeong1030@gmail.com</t>
+  </si>
+  <si>
+    <t>최유정</t>
+  </si>
+  <si>
+    <t>jyoon2233@naver.com</t>
+  </si>
+  <si>
+    <t>신정윤</t>
+  </si>
+  <si>
+    <t>chltjdnjs2421@naver.com</t>
+  </si>
+  <si>
+    <t>최서원</t>
+  </si>
+  <si>
+    <t>kter0506@naver.com</t>
+  </si>
+  <si>
+    <t>김태은</t>
+  </si>
+  <si>
+    <t>gchans0524@gmail.com</t>
+  </si>
+  <si>
+    <t>한기찬</t>
+  </si>
+  <si>
+    <t>alwnd816@gmail.com</t>
+  </si>
+  <si>
+    <t>한재은</t>
+  </si>
+  <si>
+    <t>ac3512@naver.com</t>
+  </si>
+  <si>
+    <t>김태근</t>
+  </si>
+  <si>
+    <t>tommy21940@gmail.com</t>
+  </si>
+  <si>
+    <t>양민혁</t>
+  </si>
+  <si>
+    <t>zxcod10@gmail.com</t>
+  </si>
+  <si>
+    <t>최원용</t>
+  </si>
+  <si>
+    <t>tjdehs4809@naver.com</t>
+  </si>
+  <si>
+    <t>최성돈</t>
+  </si>
+  <si>
+    <t>youmin43@naver.com</t>
+  </si>
+  <si>
+    <t>박유민</t>
   </si>
 </sst>
 </file>
@@ -2816,7 +3056,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:AD300">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:AD340">
   <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -3054,11 +3294,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD300"/>
+  <dimension ref="A1:AD340"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D321" sqref="D321"/>
+      <pane ySplit="1" topLeftCell="A298" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F353" sqref="F353"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -30691,6 +30931,3686 @@
         <v>56</v>
       </c>
     </row>
+    <row r="301" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A301" s="7">
+        <v>45570.77539988426</v>
+      </c>
+      <c r="B301" s="8" t="s">
+        <v>794</v>
+      </c>
+      <c r="C301" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="D301" s="8">
+        <v>20231539</v>
+      </c>
+      <c r="E301" s="8" t="s">
+        <v>795</v>
+      </c>
+      <c r="F301" s="8">
+        <v>3</v>
+      </c>
+      <c r="G301" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="H301" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I301" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J301" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K301" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L301" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="M301" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N301" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O301" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="P301" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q301" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="R301" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S301" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="T301" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U301" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V301" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W301" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="X301" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="Y301" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z301" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="AA301" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB301" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC301" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD301" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="302" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A302" s="4">
+        <v>45570.791212349533</v>
+      </c>
+      <c r="B302" s="5" t="s">
+        <v>796</v>
+      </c>
+      <c r="C302" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D302" s="5">
+        <v>20242314</v>
+      </c>
+      <c r="E302" s="5" t="s">
+        <v>797</v>
+      </c>
+      <c r="F302" s="5">
+        <v>3</v>
+      </c>
+      <c r="G302" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H302" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I302" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J302" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K302" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L302" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M302" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N302" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O302" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P302" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q302" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R302" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S302" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T302" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="U302" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V302" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W302" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X302" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y302" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z302" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA302" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB302" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC302" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD302" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="303" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A303" s="7">
+        <v>45570.803095439813</v>
+      </c>
+      <c r="B303" s="8" t="s">
+        <v>798</v>
+      </c>
+      <c r="C303" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D303" s="8">
+        <v>20234110</v>
+      </c>
+      <c r="E303" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="F303" s="8">
+        <v>3</v>
+      </c>
+      <c r="G303" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H303" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I303" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J303" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K303" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L303" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M303" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N303" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O303" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P303" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q303" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R303" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S303" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T303" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U303" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V303" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W303" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X303" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y303" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z303" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA303" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB303" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC303" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD303" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="304" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A304" s="4">
+        <v>45570.811618541666</v>
+      </c>
+      <c r="B304" s="5" t="s">
+        <v>800</v>
+      </c>
+      <c r="C304" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D304" s="5">
+        <v>20211630</v>
+      </c>
+      <c r="E304" s="5" t="s">
+        <v>801</v>
+      </c>
+      <c r="F304" s="5">
+        <v>3</v>
+      </c>
+      <c r="G304" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H304" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I304" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J304" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K304" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L304" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M304" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="N304" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O304" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P304" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q304" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R304" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S304" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T304" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U304" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V304" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W304" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X304" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y304" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z304" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA304" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB304" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC304" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD304" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="305" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A305" s="7">
+        <v>45570.821239467594</v>
+      </c>
+      <c r="B305" s="8" t="s">
+        <v>802</v>
+      </c>
+      <c r="C305" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D305" s="8">
+        <v>20242844</v>
+      </c>
+      <c r="E305" s="8" t="s">
+        <v>803</v>
+      </c>
+      <c r="F305" s="8">
+        <v>3</v>
+      </c>
+      <c r="G305" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H305" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I305" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J305" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K305" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L305" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M305" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N305" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O305" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P305" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q305" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="R305" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S305" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T305" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="U305" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="V305" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W305" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X305" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y305" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z305" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA305" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB305" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC305" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD305" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="306" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A306" s="4">
+        <v>45570.846249583337</v>
+      </c>
+      <c r="B306" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="C306" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="D306" s="5">
+        <v>20216716</v>
+      </c>
+      <c r="E306" s="5" t="s">
+        <v>805</v>
+      </c>
+      <c r="F306" s="5">
+        <v>3</v>
+      </c>
+      <c r="G306" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H306" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I306" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J306" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K306" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L306" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M306" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N306" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O306" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P306" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q306" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R306" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S306" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T306" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U306" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V306" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W306" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X306" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y306" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z306" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA306" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB306" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC306" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD306" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="307" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A307" s="7">
+        <v>45570.846548298607</v>
+      </c>
+      <c r="B307" s="8" t="s">
+        <v>806</v>
+      </c>
+      <c r="C307" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="D307" s="8">
+        <v>20241236</v>
+      </c>
+      <c r="E307" s="8" t="s">
+        <v>807</v>
+      </c>
+      <c r="F307" s="8">
+        <v>2</v>
+      </c>
+      <c r="G307" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="H307" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I307" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J307" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="K307" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L307" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M307" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N307" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O307" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P307" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q307" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R307" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="S307" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="T307" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U307" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V307" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="W307" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="X307" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y307" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z307" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA307" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB307" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC307" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD307" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="308" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A308" s="4">
+        <v>45570.848092256943</v>
+      </c>
+      <c r="B308" s="5" t="s">
+        <v>808</v>
+      </c>
+      <c r="C308" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D308" s="5">
+        <v>20241047</v>
+      </c>
+      <c r="E308" s="5" t="s">
+        <v>809</v>
+      </c>
+      <c r="F308" s="5">
+        <v>3</v>
+      </c>
+      <c r="G308" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H308" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I308" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J308" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K308" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L308" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M308" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="N308" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O308" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P308" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q308" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R308" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S308" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T308" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U308" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V308" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="W308" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X308" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y308" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z308" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA308" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB308" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC308" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD308" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="309" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A309" s="7">
+        <v>45570.859636493056</v>
+      </c>
+      <c r="B309" s="8" t="s">
+        <v>810</v>
+      </c>
+      <c r="C309" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D309" s="8">
+        <v>20245259</v>
+      </c>
+      <c r="E309" s="8" t="s">
+        <v>811</v>
+      </c>
+      <c r="F309" s="8">
+        <v>3</v>
+      </c>
+      <c r="G309" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H309" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I309" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J309" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K309" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L309" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M309" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="N309" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O309" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P309" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q309" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R309" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S309" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T309" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="U309" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="V309" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W309" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X309" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y309" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z309" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA309" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB309" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC309" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD309" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="310" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A310" s="4">
+        <v>45570.86919626157</v>
+      </c>
+      <c r="B310" s="5" t="s">
+        <v>812</v>
+      </c>
+      <c r="C310" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D310" s="5">
+        <v>20241095</v>
+      </c>
+      <c r="E310" s="5" t="s">
+        <v>813</v>
+      </c>
+      <c r="F310" s="5">
+        <v>3</v>
+      </c>
+      <c r="G310" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H310" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I310" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J310" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K310" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L310" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M310" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N310" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O310" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P310" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q310" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R310" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S310" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T310" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="U310" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V310" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W310" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X310" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y310" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z310" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA310" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB310" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC310" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD310" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="311" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A311" s="7">
+        <v>45570.870069699071</v>
+      </c>
+      <c r="B311" s="8" t="s">
+        <v>814</v>
+      </c>
+      <c r="C311" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="D311" s="8">
+        <v>20246628</v>
+      </c>
+      <c r="E311" s="8" t="s">
+        <v>815</v>
+      </c>
+      <c r="F311" s="8">
+        <v>3</v>
+      </c>
+      <c r="G311" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H311" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I311" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J311" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K311" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L311" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="M311" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N311" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O311" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P311" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q311" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="R311" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S311" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T311" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U311" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V311" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W311" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X311" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y311" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z311" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA311" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB311" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC311" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD311" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="312" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A312" s="4">
+        <v>45570.879679699079</v>
+      </c>
+      <c r="B312" s="5" t="s">
+        <v>816</v>
+      </c>
+      <c r="C312" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="D312" s="5">
+        <v>20227022</v>
+      </c>
+      <c r="E312" s="5" t="s">
+        <v>817</v>
+      </c>
+      <c r="F312" s="5">
+        <v>3</v>
+      </c>
+      <c r="G312" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H312" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I312" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J312" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K312" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L312" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="M312" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="N312" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O312" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="P312" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q312" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R312" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="S312" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="T312" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U312" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="V312" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W312" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X312" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y312" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z312" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AA312" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB312" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC312" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD312" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="313" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A313" s="7">
+        <v>45570.880150949073</v>
+      </c>
+      <c r="B313" s="8" t="s">
+        <v>818</v>
+      </c>
+      <c r="C313" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D313" s="8">
+        <v>20243903</v>
+      </c>
+      <c r="E313" s="8" t="s">
+        <v>819</v>
+      </c>
+      <c r="F313" s="8">
+        <v>3</v>
+      </c>
+      <c r="G313" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H313" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I313" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J313" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K313" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L313" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M313" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N313" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O313" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P313" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q313" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R313" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S313" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T313" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="U313" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="V313" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W313" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X313" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y313" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z313" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA313" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB313" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC313" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD313" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="314" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A314" s="4">
+        <v>45570.884164953706</v>
+      </c>
+      <c r="B314" s="5" t="s">
+        <v>820</v>
+      </c>
+      <c r="C314" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D314" s="5">
+        <v>20242323</v>
+      </c>
+      <c r="E314" s="5" t="s">
+        <v>821</v>
+      </c>
+      <c r="F314" s="5">
+        <v>3</v>
+      </c>
+      <c r="G314" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H314" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I314" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J314" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K314" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L314" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M314" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N314" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O314" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P314" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q314" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R314" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S314" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T314" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U314" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V314" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W314" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X314" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y314" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z314" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA314" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB314" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC314" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD314" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="315" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A315" s="7">
+        <v>45570.887954004633</v>
+      </c>
+      <c r="B315" s="8" t="s">
+        <v>822</v>
+      </c>
+      <c r="C315" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D315" s="8">
+        <v>20172719</v>
+      </c>
+      <c r="E315" s="8" t="s">
+        <v>823</v>
+      </c>
+      <c r="F315" s="8">
+        <v>3</v>
+      </c>
+      <c r="G315" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H315" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I315" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J315" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K315" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L315" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M315" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N315" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O315" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P315" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q315" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R315" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S315" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T315" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U315" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V315" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W315" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X315" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y315" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z315" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA315" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB315" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC315" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD315" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="316" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A316" s="4">
+        <v>45570.892073993055</v>
+      </c>
+      <c r="B316" s="5" t="s">
+        <v>824</v>
+      </c>
+      <c r="C316" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D316" s="5">
+        <v>20242751</v>
+      </c>
+      <c r="E316" s="5" t="s">
+        <v>825</v>
+      </c>
+      <c r="F316" s="5">
+        <v>3</v>
+      </c>
+      <c r="G316" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H316" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I316" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J316" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K316" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L316" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M316" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N316" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O316" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P316" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q316" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R316" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S316" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T316" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U316" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V316" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W316" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X316" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y316" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z316" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA316" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB316" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC316" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD316" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="317" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A317" s="7">
+        <v>45570.897373148153</v>
+      </c>
+      <c r="B317" s="8" t="s">
+        <v>826</v>
+      </c>
+      <c r="C317" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D317" s="8">
+        <v>20242358</v>
+      </c>
+      <c r="E317" s="8" t="s">
+        <v>827</v>
+      </c>
+      <c r="F317" s="8">
+        <v>3</v>
+      </c>
+      <c r="G317" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="H317" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I317" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="J317" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="K317" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="L317" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="M317" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N317" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O317" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="P317" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q317" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="R317" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="S317" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T317" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U317" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="V317" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W317" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="X317" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y317" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z317" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA317" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB317" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC317" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="AD317" s="9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="318" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A318" s="4">
+        <v>45570.915063692126</v>
+      </c>
+      <c r="B318" s="5" t="s">
+        <v>828</v>
+      </c>
+      <c r="C318" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="D318" s="5">
+        <v>20246776</v>
+      </c>
+      <c r="E318" s="5" t="s">
+        <v>829</v>
+      </c>
+      <c r="F318" s="5">
+        <v>3</v>
+      </c>
+      <c r="G318" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H318" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I318" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J318" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K318" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L318" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M318" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="N318" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O318" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P318" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q318" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R318" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S318" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T318" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U318" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V318" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W318" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X318" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y318" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z318" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA318" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB318" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC318" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD318" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="319" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A319" s="7">
+        <v>45570.91820511574</v>
+      </c>
+      <c r="B319" s="8" t="s">
+        <v>830</v>
+      </c>
+      <c r="C319" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D319" s="8">
+        <v>20191226</v>
+      </c>
+      <c r="E319" s="8" t="s">
+        <v>831</v>
+      </c>
+      <c r="F319" s="8">
+        <v>3</v>
+      </c>
+      <c r="G319" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H319" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I319" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J319" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="K319" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L319" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M319" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N319" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O319" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P319" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q319" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R319" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S319" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T319" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="U319" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V319" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W319" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X319" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y319" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z319" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA319" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB319" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC319" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD319" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="320" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A320" s="4">
+        <v>45570.919459537035</v>
+      </c>
+      <c r="B320" s="5" t="s">
+        <v>832</v>
+      </c>
+      <c r="C320" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D320" s="5">
+        <v>20245207</v>
+      </c>
+      <c r="E320" s="5" t="s">
+        <v>833</v>
+      </c>
+      <c r="F320" s="5">
+        <v>3</v>
+      </c>
+      <c r="G320" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H320" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I320" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J320" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K320" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L320" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M320" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N320" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O320" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P320" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q320" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R320" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S320" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T320" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U320" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V320" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W320" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X320" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y320" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z320" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA320" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB320" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC320" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD320" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="321" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A321" s="7">
+        <v>45570.929818854165</v>
+      </c>
+      <c r="B321" s="8" t="s">
+        <v>834</v>
+      </c>
+      <c r="C321" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D321" s="8">
+        <v>20244126</v>
+      </c>
+      <c r="E321" s="8" t="s">
+        <v>835</v>
+      </c>
+      <c r="F321" s="8">
+        <v>3</v>
+      </c>
+      <c r="G321" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="H321" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I321" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J321" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="K321" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L321" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="M321" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="N321" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O321" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P321" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q321" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R321" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S321" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="T321" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="U321" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V321" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="W321" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X321" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y321" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z321" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA321" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB321" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC321" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD321" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="322" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A322" s="4">
+        <v>45570.944059629634</v>
+      </c>
+      <c r="B322" s="5" t="s">
+        <v>836</v>
+      </c>
+      <c r="C322" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D322" s="5">
+        <v>20242347</v>
+      </c>
+      <c r="E322" s="5" t="s">
+        <v>837</v>
+      </c>
+      <c r="F322" s="5">
+        <v>3</v>
+      </c>
+      <c r="G322" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H322" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I322" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J322" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K322" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L322" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M322" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N322" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O322" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P322" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q322" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R322" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S322" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T322" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U322" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V322" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W322" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X322" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y322" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z322" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA322" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB322" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC322" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD322" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="323" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A323" s="7">
+        <v>45570.986215115743</v>
+      </c>
+      <c r="B323" s="8" t="s">
+        <v>838</v>
+      </c>
+      <c r="C323" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="D323" s="8">
+        <v>20246648</v>
+      </c>
+      <c r="E323" s="8" t="s">
+        <v>839</v>
+      </c>
+      <c r="F323" s="8">
+        <v>3</v>
+      </c>
+      <c r="G323" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="H323" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I323" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="J323" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="K323" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="L323" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M323" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N323" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O323" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P323" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q323" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="R323" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="S323" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="T323" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U323" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="V323" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="W323" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X323" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y323" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z323" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="AA323" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB323" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC323" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="AD323" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="324" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A324" s="4">
+        <v>45570.995128344905</v>
+      </c>
+      <c r="B324" s="5" t="s">
+        <v>840</v>
+      </c>
+      <c r="C324" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D324" s="5">
+        <v>20242128</v>
+      </c>
+      <c r="E324" s="5" t="s">
+        <v>841</v>
+      </c>
+      <c r="F324" s="5">
+        <v>3</v>
+      </c>
+      <c r="G324" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="H324" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I324" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J324" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K324" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="L324" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M324" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="N324" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O324" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P324" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q324" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R324" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S324" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T324" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U324" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V324" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W324" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X324" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y324" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z324" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA324" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB324" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC324" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD324" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="325" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A325" s="7">
+        <v>45571.007126458338</v>
+      </c>
+      <c r="B325" s="8" t="s">
+        <v>842</v>
+      </c>
+      <c r="C325" s="8" t="s">
+        <v>762</v>
+      </c>
+      <c r="D325" s="8">
+        <v>20242925</v>
+      </c>
+      <c r="E325" s="8" t="s">
+        <v>843</v>
+      </c>
+      <c r="F325" s="8">
+        <v>3</v>
+      </c>
+      <c r="G325" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H325" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I325" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J325" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K325" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L325" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M325" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N325" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O325" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P325" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q325" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R325" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S325" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T325" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="U325" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V325" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W325" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X325" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y325" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z325" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA325" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB325" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC325" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD325" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="326" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A326" s="4">
+        <v>45571.007742106478</v>
+      </c>
+      <c r="B326" s="5" t="s">
+        <v>844</v>
+      </c>
+      <c r="C326" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D326" s="5">
+        <v>20222933</v>
+      </c>
+      <c r="E326" s="5" t="s">
+        <v>845</v>
+      </c>
+      <c r="F326" s="5">
+        <v>3</v>
+      </c>
+      <c r="G326" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H326" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I326" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J326" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K326" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L326" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M326" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N326" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O326" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P326" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q326" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R326" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S326" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T326" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U326" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V326" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W326" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X326" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y326" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z326" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA326" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB326" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC326" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD326" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="327" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A327" s="7">
+        <v>45571.012530520835</v>
+      </c>
+      <c r="B327" s="8" t="s">
+        <v>846</v>
+      </c>
+      <c r="C327" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D327" s="8">
+        <v>20217087</v>
+      </c>
+      <c r="E327" s="8" t="s">
+        <v>847</v>
+      </c>
+      <c r="F327" s="8">
+        <v>3</v>
+      </c>
+      <c r="G327" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H327" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I327" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J327" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K327" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L327" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M327" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N327" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O327" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P327" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q327" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R327" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S327" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T327" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U327" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V327" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W327" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X327" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y327" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z327" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA327" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB327" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC327" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD327" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="328" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A328" s="4">
+        <v>45571.022266192129</v>
+      </c>
+      <c r="B328" s="5" t="s">
+        <v>848</v>
+      </c>
+      <c r="C328" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D328" s="5">
+        <v>20242336</v>
+      </c>
+      <c r="E328" s="5" t="s">
+        <v>849</v>
+      </c>
+      <c r="F328" s="5">
+        <v>3</v>
+      </c>
+      <c r="G328" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H328" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I328" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J328" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K328" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L328" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M328" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N328" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O328" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P328" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q328" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R328" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S328" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T328" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="U328" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V328" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W328" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X328" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y328" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z328" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA328" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB328" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC328" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD328" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="329" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A329" s="7">
+        <v>45571.034601712963</v>
+      </c>
+      <c r="B329" s="8" t="s">
+        <v>850</v>
+      </c>
+      <c r="C329" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="D329" s="8">
+        <v>20211523</v>
+      </c>
+      <c r="E329" s="8" t="s">
+        <v>851</v>
+      </c>
+      <c r="F329" s="8">
+        <v>3</v>
+      </c>
+      <c r="G329" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H329" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I329" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J329" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K329" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L329" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M329" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N329" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O329" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P329" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q329" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="R329" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S329" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T329" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U329" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V329" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W329" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X329" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y329" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z329" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA329" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB329" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC329" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="AD329" s="9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="330" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A330" s="4">
+        <v>45571.038926504625</v>
+      </c>
+      <c r="B330" s="5" t="s">
+        <v>852</v>
+      </c>
+      <c r="C330" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="D330" s="5">
+        <v>20232637</v>
+      </c>
+      <c r="E330" s="5" t="s">
+        <v>853</v>
+      </c>
+      <c r="F330" s="5">
+        <v>3</v>
+      </c>
+      <c r="G330" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H330" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I330" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J330" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K330" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L330" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M330" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N330" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O330" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P330" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q330" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R330" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S330" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T330" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U330" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V330" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W330" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X330" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y330" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z330" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA330" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB330" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC330" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD330" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="331" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A331" s="7">
+        <v>45571.046686562499</v>
+      </c>
+      <c r="B331" s="8" t="s">
+        <v>854</v>
+      </c>
+      <c r="C331" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D331" s="8">
+        <v>20245190</v>
+      </c>
+      <c r="E331" s="8" t="s">
+        <v>855</v>
+      </c>
+      <c r="F331" s="8">
+        <v>3</v>
+      </c>
+      <c r="G331" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H331" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I331" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J331" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K331" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L331" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M331" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N331" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O331" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P331" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q331" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R331" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S331" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T331" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="U331" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V331" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W331" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X331" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y331" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z331" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA331" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB331" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC331" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD331" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="332" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A332" s="4">
+        <v>45571.049937187505</v>
+      </c>
+      <c r="B332" s="5" t="s">
+        <v>856</v>
+      </c>
+      <c r="C332" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D332" s="5">
+        <v>20242848</v>
+      </c>
+      <c r="E332" s="5" t="s">
+        <v>857</v>
+      </c>
+      <c r="F332" s="5">
+        <v>3</v>
+      </c>
+      <c r="G332" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="H332" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I332" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J332" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K332" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="L332" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M332" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N332" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O332" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P332" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q332" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R332" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S332" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T332" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U332" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V332" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="W332" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X332" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y332" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z332" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA332" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB332" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC332" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD332" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="333" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A333" s="7">
+        <v>45571.064924050923</v>
+      </c>
+      <c r="B333" s="8" t="s">
+        <v>858</v>
+      </c>
+      <c r="C333" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D333" s="8">
+        <v>20243813</v>
+      </c>
+      <c r="E333" s="8" t="s">
+        <v>859</v>
+      </c>
+      <c r="F333" s="8">
+        <v>3</v>
+      </c>
+      <c r="G333" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H333" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I333" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J333" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K333" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L333" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M333" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N333" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O333" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P333" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q333" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R333" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S333" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T333" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U333" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V333" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W333" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X333" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y333" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z333" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA333" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB333" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC333" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD333" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="334" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A334" s="4">
+        <v>45571.074850150464</v>
+      </c>
+      <c r="B334" s="5" t="s">
+        <v>860</v>
+      </c>
+      <c r="C334" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D334" s="5">
+        <v>20244152</v>
+      </c>
+      <c r="E334" s="5" t="s">
+        <v>861</v>
+      </c>
+      <c r="F334" s="5">
+        <v>3</v>
+      </c>
+      <c r="G334" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H334" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I334" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J334" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K334" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L334" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M334" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="N334" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O334" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P334" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q334" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R334" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="S334" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T334" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="U334" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V334" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W334" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X334" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y334" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z334" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA334" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB334" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC334" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="AD334" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="335" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A335" s="7">
+        <v>45571.088335509259</v>
+      </c>
+      <c r="B335" s="8" t="s">
+        <v>862</v>
+      </c>
+      <c r="C335" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D335" s="8">
+        <v>20233060</v>
+      </c>
+      <c r="E335" s="8" t="s">
+        <v>863</v>
+      </c>
+      <c r="F335" s="8">
+        <v>3</v>
+      </c>
+      <c r="G335" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H335" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I335" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J335" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K335" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L335" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M335" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="N335" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O335" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P335" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q335" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R335" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S335" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T335" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U335" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V335" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W335" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X335" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y335" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z335" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA335" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB335" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC335" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD335" s="9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="336" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A336" s="4">
+        <v>45571.092030081018</v>
+      </c>
+      <c r="B336" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="C336" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="D336" s="5">
+        <v>20216609</v>
+      </c>
+      <c r="E336" s="5" t="s">
+        <v>865</v>
+      </c>
+      <c r="F336" s="5">
+        <v>3</v>
+      </c>
+      <c r="G336" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H336" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I336" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J336" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K336" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L336" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M336" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N336" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O336" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P336" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q336" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R336" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S336" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T336" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U336" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="V336" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W336" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X336" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y336" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z336" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA336" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB336" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC336" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD336" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="337" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A337" s="7">
+        <v>45571.107449930554</v>
+      </c>
+      <c r="B337" s="8" t="s">
+        <v>866</v>
+      </c>
+      <c r="C337" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D337" s="8">
+        <v>20241054</v>
+      </c>
+      <c r="E337" s="8" t="s">
+        <v>867</v>
+      </c>
+      <c r="F337" s="8">
+        <v>3</v>
+      </c>
+      <c r="G337" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H337" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I337" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J337" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K337" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="L337" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M337" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N337" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O337" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P337" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q337" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R337" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S337" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T337" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U337" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V337" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W337" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X337" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y337" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z337" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA337" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB337" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC337" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD337" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="338" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A338" s="4">
+        <v>45571.1124715162</v>
+      </c>
+      <c r="B338" s="5" t="s">
+        <v>868</v>
+      </c>
+      <c r="C338" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D338" s="5">
+        <v>20217135</v>
+      </c>
+      <c r="E338" s="5" t="s">
+        <v>869</v>
+      </c>
+      <c r="F338" s="5">
+        <v>3</v>
+      </c>
+      <c r="G338" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H338" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I338" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J338" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K338" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L338" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M338" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N338" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O338" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="P338" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q338" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R338" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="S338" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="T338" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="U338" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V338" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="W338" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="X338" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="Y338" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z338" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA338" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB338" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="AC338" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD338" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="339" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A339" s="7">
+        <v>45571.136986238431</v>
+      </c>
+      <c r="B339" s="8" t="s">
+        <v>870</v>
+      </c>
+      <c r="C339" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="D339" s="8">
+        <v>20201103</v>
+      </c>
+      <c r="E339" s="8" t="s">
+        <v>871</v>
+      </c>
+      <c r="F339" s="8">
+        <v>3</v>
+      </c>
+      <c r="G339" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H339" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I339" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J339" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K339" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L339" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M339" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N339" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O339" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P339" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q339" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R339" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S339" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T339" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U339" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V339" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W339" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X339" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y339" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z339" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA339" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB339" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC339" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD339" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="340" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A340" s="16">
+        <v>45571.243750324073</v>
+      </c>
+      <c r="B340" s="17" t="s">
+        <v>872</v>
+      </c>
+      <c r="C340" s="17" t="s">
+        <v>372</v>
+      </c>
+      <c r="D340" s="17">
+        <v>20246728</v>
+      </c>
+      <c r="E340" s="17" t="s">
+        <v>873</v>
+      </c>
+      <c r="F340" s="17">
+        <v>3</v>
+      </c>
+      <c r="G340" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H340" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="I340" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="J340" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="K340" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="L340" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="M340" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="N340" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="O340" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="P340" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q340" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="R340" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="S340" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="T340" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="U340" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="V340" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="W340" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="X340" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y340" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z340" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA340" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB340" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC340" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD340" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
literacy, 240930 modified 10
</commit_message>
<xml_diff>
--- a/R/data/literacy_240930.xlsx
+++ b/R/data/literacy_240930.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AD7725-A9D2-D64E-90F6-748C6282BC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2B10D0-F7A9-A04B-96BD-4E27A478BE06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50400" yWindow="1360" windowWidth="44800" windowHeight="24700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9183" uniqueCount="874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9993" uniqueCount="937">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -2642,6 +2642,195 @@
   </si>
   <si>
     <t>박유민</t>
+  </si>
+  <si>
+    <t>p20236727@gmail.com</t>
+  </si>
+  <si>
+    <t>박진서</t>
+  </si>
+  <si>
+    <t>vcx76613@gmail.com</t>
+  </si>
+  <si>
+    <t>황인태</t>
+  </si>
+  <si>
+    <t>minsung5342@naver.com</t>
+  </si>
+  <si>
+    <t>doheehana@naver.com</t>
+  </si>
+  <si>
+    <t>김도희</t>
+  </si>
+  <si>
+    <t>wnsrl2498@naver.com</t>
+  </si>
+  <si>
+    <t>김준기</t>
+  </si>
+  <si>
+    <t>dlaehdghks123@gmail.com</t>
+  </si>
+  <si>
+    <t>임동환</t>
+  </si>
+  <si>
+    <t>shasha4321@naver.com</t>
+  </si>
+  <si>
+    <t>경영학</t>
+  </si>
+  <si>
+    <t>정다영</t>
+  </si>
+  <si>
+    <t>sumine0601@naver.com</t>
+  </si>
+  <si>
+    <t>장수민</t>
+  </si>
+  <si>
+    <t>whrudghks030604@naver.com</t>
+  </si>
+  <si>
+    <t>조경환</t>
+  </si>
+  <si>
+    <t>leedowon567@naver.com</t>
+  </si>
+  <si>
+    <t>이도원</t>
+  </si>
+  <si>
+    <t>sshee718@gmail.com</t>
+  </si>
+  <si>
+    <t>권도운</t>
+  </si>
+  <si>
+    <t>lattace05@gmail.com</t>
+  </si>
+  <si>
+    <t>최동희</t>
+  </si>
+  <si>
+    <t>r67890@naver.com</t>
+  </si>
+  <si>
+    <t>이규형</t>
+  </si>
+  <si>
+    <t>jiminn101777@gmail.com</t>
+  </si>
+  <si>
+    <t>권지민</t>
+  </si>
+  <si>
+    <t>dlakrp731@gmail.com</t>
+  </si>
+  <si>
+    <t>콘텐츠it</t>
+  </si>
+  <si>
+    <t>이준수</t>
+  </si>
+  <si>
+    <t>twenty__dec@naver.com</t>
+  </si>
+  <si>
+    <t>채희주</t>
+  </si>
+  <si>
+    <t>wldus0859@gmail.com</t>
+  </si>
+  <si>
+    <t>박지연</t>
+  </si>
+  <si>
+    <t>chetbaker22@naver.com</t>
+  </si>
+  <si>
+    <t>철학전공</t>
+  </si>
+  <si>
+    <t>김채원</t>
+  </si>
+  <si>
+    <t>guj2205146@gmail.com</t>
+  </si>
+  <si>
+    <t>강의주</t>
+  </si>
+  <si>
+    <t>yuvin0612@naver.com</t>
+  </si>
+  <si>
+    <t>장유빈</t>
+  </si>
+  <si>
+    <t>simyenho8562@gmail.com</t>
+  </si>
+  <si>
+    <t>심연호</t>
+  </si>
+  <si>
+    <t>h20191240@glab.hallym.ac.kr</t>
+  </si>
+  <si>
+    <t>홍이래</t>
+  </si>
+  <si>
+    <t>hyeonjin0976@gmail.com</t>
+  </si>
+  <si>
+    <t>류현진</t>
+  </si>
+  <si>
+    <t>jangjunhyeok1001@naver.com</t>
+  </si>
+  <si>
+    <t>반도체디스플레이 스쿨</t>
+  </si>
+  <si>
+    <t>장준혁</t>
+  </si>
+  <si>
+    <t>jjy021026@gmail.com</t>
+  </si>
+  <si>
+    <t>전지환</t>
+  </si>
+  <si>
+    <t>applehanul@naver.com</t>
+  </si>
+  <si>
+    <t>신하늘</t>
+  </si>
+  <si>
+    <t>ncu11069@naver.com</t>
+  </si>
+  <si>
+    <t>이규민</t>
+  </si>
+  <si>
+    <t>buj5195193@naver.com</t>
+  </si>
+  <si>
+    <t>백유진</t>
+  </si>
+  <si>
+    <t>sk2000tyr@naver.com</t>
+  </si>
+  <si>
+    <t>이지한</t>
+  </si>
+  <si>
+    <t>skyhaneul0910@naver.com</t>
+  </si>
+  <si>
+    <t>권하늘</t>
   </si>
 </sst>
 </file>
@@ -3056,7 +3245,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:AD340">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:AD370">
   <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -3294,11 +3483,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD340"/>
+  <dimension ref="A1:AD370"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A298" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F353" sqref="F353"/>
+      <pane ySplit="1" topLeftCell="A327" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F382" sqref="F382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -34611,6 +34800,2766 @@
         <v>56</v>
       </c>
     </row>
+    <row r="341" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A341" s="7">
+        <v>45571.364452442125</v>
+      </c>
+      <c r="B341" s="8" t="s">
+        <v>874</v>
+      </c>
+      <c r="C341" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="D341" s="8">
+        <v>20236727</v>
+      </c>
+      <c r="E341" s="8" t="s">
+        <v>875</v>
+      </c>
+      <c r="F341" s="8">
+        <v>3</v>
+      </c>
+      <c r="G341" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H341" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I341" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J341" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K341" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L341" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="M341" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N341" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O341" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P341" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q341" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R341" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S341" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T341" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="U341" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V341" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W341" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X341" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y341" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z341" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="AA341" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB341" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC341" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD341" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="342" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A342" s="4">
+        <v>45571.38792552083</v>
+      </c>
+      <c r="B342" s="5" t="s">
+        <v>876</v>
+      </c>
+      <c r="C342" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D342" s="5">
+        <v>20246306</v>
+      </c>
+      <c r="E342" s="5" t="s">
+        <v>877</v>
+      </c>
+      <c r="F342" s="5">
+        <v>3</v>
+      </c>
+      <c r="G342" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H342" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I342" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J342" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K342" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="L342" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M342" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="N342" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O342" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="P342" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q342" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R342" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="S342" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="T342" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U342" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="V342" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="W342" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="X342" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y342" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z342" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AA342" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB342" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC342" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD342" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="343" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A343" s="7">
+        <v>45571.432436701391</v>
+      </c>
+      <c r="B343" s="8" t="s">
+        <v>878</v>
+      </c>
+      <c r="C343" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="D343" s="8">
+        <v>20232311</v>
+      </c>
+      <c r="E343" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="F343" s="8">
+        <v>3</v>
+      </c>
+      <c r="G343" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H343" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I343" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J343" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K343" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L343" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M343" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N343" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O343" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P343" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q343" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R343" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S343" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T343" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U343" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V343" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W343" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X343" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y343" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z343" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA343" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB343" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC343" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD343" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="344" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A344" s="4">
+        <v>45571.449635729165</v>
+      </c>
+      <c r="B344" s="5" t="s">
+        <v>879</v>
+      </c>
+      <c r="C344" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D344" s="5">
+        <v>20246215</v>
+      </c>
+      <c r="E344" s="5" t="s">
+        <v>880</v>
+      </c>
+      <c r="F344" s="5">
+        <v>3</v>
+      </c>
+      <c r="G344" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H344" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I344" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J344" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K344" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L344" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M344" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N344" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O344" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P344" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q344" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R344" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S344" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T344" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="U344" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V344" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W344" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X344" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y344" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z344" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA344" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB344" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC344" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="AD344" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="345" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A345" s="7">
+        <v>45571.501602731485</v>
+      </c>
+      <c r="B345" s="8" t="s">
+        <v>881</v>
+      </c>
+      <c r="C345" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D345" s="8">
+        <v>20227093</v>
+      </c>
+      <c r="E345" s="8" t="s">
+        <v>882</v>
+      </c>
+      <c r="F345" s="8">
+        <v>2</v>
+      </c>
+      <c r="G345" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H345" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I345" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J345" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="K345" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L345" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M345" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N345" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O345" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P345" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q345" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R345" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S345" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T345" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U345" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V345" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W345" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X345" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y345" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z345" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA345" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB345" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC345" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="AD345" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="346" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A346" s="4">
+        <v>45571.516520648147</v>
+      </c>
+      <c r="B346" s="5" t="s">
+        <v>883</v>
+      </c>
+      <c r="C346" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D346" s="5">
+        <v>20213533</v>
+      </c>
+      <c r="E346" s="5" t="s">
+        <v>884</v>
+      </c>
+      <c r="F346" s="5">
+        <v>3</v>
+      </c>
+      <c r="G346" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H346" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I346" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J346" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="K346" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L346" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M346" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N346" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O346" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P346" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q346" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R346" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S346" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T346" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U346" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V346" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W346" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X346" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y346" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z346" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA346" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB346" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC346" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD346" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="347" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A347" s="7">
+        <v>45571.534782256946</v>
+      </c>
+      <c r="B347" s="8" t="s">
+        <v>885</v>
+      </c>
+      <c r="C347" s="8" t="s">
+        <v>886</v>
+      </c>
+      <c r="D347" s="8">
+        <v>20213035</v>
+      </c>
+      <c r="E347" s="8" t="s">
+        <v>887</v>
+      </c>
+      <c r="F347" s="8">
+        <v>3</v>
+      </c>
+      <c r="G347" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H347" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I347" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J347" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K347" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L347" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M347" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N347" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O347" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P347" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q347" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R347" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S347" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T347" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="U347" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V347" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W347" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X347" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y347" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z347" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA347" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB347" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC347" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD347" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="348" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A348" s="4">
+        <v>45571.552414502316</v>
+      </c>
+      <c r="B348" s="5" t="s">
+        <v>888</v>
+      </c>
+      <c r="C348" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="D348" s="5">
+        <v>20202637</v>
+      </c>
+      <c r="E348" s="5" t="s">
+        <v>889</v>
+      </c>
+      <c r="F348" s="5">
+        <v>3</v>
+      </c>
+      <c r="G348" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H348" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I348" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J348" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K348" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L348" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M348" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="N348" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O348" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P348" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q348" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R348" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S348" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T348" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="U348" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V348" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W348" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X348" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y348" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z348" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA348" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB348" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC348" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD348" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="349" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A349" s="7">
+        <v>45571.557763229168</v>
+      </c>
+      <c r="B349" s="8" t="s">
+        <v>890</v>
+      </c>
+      <c r="C349" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D349" s="8">
+        <v>20243955</v>
+      </c>
+      <c r="E349" s="8" t="s">
+        <v>891</v>
+      </c>
+      <c r="F349" s="8">
+        <v>3</v>
+      </c>
+      <c r="G349" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H349" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I349" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J349" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K349" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L349" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M349" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N349" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O349" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P349" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q349" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R349" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S349" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T349" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U349" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="V349" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W349" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X349" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y349" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z349" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA349" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB349" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC349" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD349" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="350" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A350" s="4">
+        <v>45571.562407696758</v>
+      </c>
+      <c r="B350" s="5" t="s">
+        <v>892</v>
+      </c>
+      <c r="C350" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D350" s="5">
+        <v>20211625</v>
+      </c>
+      <c r="E350" s="5" t="s">
+        <v>893</v>
+      </c>
+      <c r="F350" s="5">
+        <v>3</v>
+      </c>
+      <c r="G350" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H350" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I350" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J350" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K350" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L350" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M350" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N350" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O350" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P350" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q350" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R350" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S350" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T350" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U350" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V350" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W350" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X350" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y350" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z350" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA350" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB350" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC350" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD350" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="351" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A351" s="7">
+        <v>45571.570918645833</v>
+      </c>
+      <c r="B351" s="8" t="s">
+        <v>894</v>
+      </c>
+      <c r="C351" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D351" s="8">
+        <v>20243702</v>
+      </c>
+      <c r="E351" s="8" t="s">
+        <v>895</v>
+      </c>
+      <c r="F351" s="8">
+        <v>3</v>
+      </c>
+      <c r="G351" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="H351" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I351" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J351" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K351" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L351" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M351" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N351" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O351" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P351" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q351" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R351" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="S351" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="T351" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U351" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="V351" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="W351" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X351" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y351" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z351" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA351" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB351" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC351" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD351" s="9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="352" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A352" s="4">
+        <v>45571.577309629633</v>
+      </c>
+      <c r="B352" s="5" t="s">
+        <v>896</v>
+      </c>
+      <c r="C352" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="D352" s="5">
+        <v>20242439</v>
+      </c>
+      <c r="E352" s="5" t="s">
+        <v>897</v>
+      </c>
+      <c r="F352" s="5">
+        <v>3</v>
+      </c>
+      <c r="G352" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H352" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I352" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J352" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K352" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L352" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M352" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N352" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O352" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P352" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q352" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R352" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S352" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T352" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U352" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V352" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W352" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X352" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y352" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z352" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA352" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB352" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC352" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD352" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="353" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A353" s="7">
+        <v>45571.581621087964</v>
+      </c>
+      <c r="B353" s="8" t="s">
+        <v>898</v>
+      </c>
+      <c r="C353" s="8" t="s">
+        <v>684</v>
+      </c>
+      <c r="D353" s="8">
+        <v>20205217</v>
+      </c>
+      <c r="E353" s="8" t="s">
+        <v>899</v>
+      </c>
+      <c r="F353" s="8">
+        <v>3</v>
+      </c>
+      <c r="G353" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H353" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I353" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J353" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="K353" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L353" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M353" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N353" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O353" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P353" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q353" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R353" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S353" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T353" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="U353" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V353" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W353" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X353" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y353" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z353" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA353" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB353" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC353" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="AD353" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="354" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A354" s="16">
+        <v>45571.594766620372</v>
+      </c>
+      <c r="B354" s="17" t="s">
+        <v>900</v>
+      </c>
+      <c r="C354" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="D354" s="17">
+        <v>20242306</v>
+      </c>
+      <c r="E354" s="17" t="s">
+        <v>901</v>
+      </c>
+      <c r="F354" s="17">
+        <v>3</v>
+      </c>
+      <c r="G354" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H354" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="I354" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="J354" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="K354" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="L354" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="M354" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="N354" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="O354" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="P354" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q354" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="R354" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="S354" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="T354" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="U354" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="V354" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="W354" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="X354" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y354" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z354" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA354" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB354" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC354" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD354" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="355" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A355" s="7">
+        <v>45571.602286990739</v>
+      </c>
+      <c r="B355" s="8" t="s">
+        <v>902</v>
+      </c>
+      <c r="C355" s="8" t="s">
+        <v>903</v>
+      </c>
+      <c r="D355" s="8">
+        <v>20195225</v>
+      </c>
+      <c r="E355" s="8" t="s">
+        <v>904</v>
+      </c>
+      <c r="F355" s="8">
+        <v>3</v>
+      </c>
+      <c r="G355" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H355" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I355" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J355" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="K355" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L355" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M355" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N355" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O355" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P355" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q355" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R355" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S355" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T355" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U355" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V355" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W355" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X355" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y355" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z355" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA355" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB355" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC355" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD355" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="356" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A356" s="4">
+        <v>45571.620481712962</v>
+      </c>
+      <c r="B356" s="5" t="s">
+        <v>905</v>
+      </c>
+      <c r="C356" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D356" s="5">
+        <v>20243959</v>
+      </c>
+      <c r="E356" s="5" t="s">
+        <v>906</v>
+      </c>
+      <c r="F356" s="5">
+        <v>3</v>
+      </c>
+      <c r="G356" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H356" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I356" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="J356" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K356" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L356" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M356" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N356" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O356" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P356" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q356" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R356" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S356" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T356" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U356" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V356" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="W356" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X356" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y356" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z356" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA356" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB356" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC356" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="AD356" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="357" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A357" s="7">
+        <v>45571.629515578708</v>
+      </c>
+      <c r="B357" s="8" t="s">
+        <v>907</v>
+      </c>
+      <c r="C357" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="D357" s="8">
+        <v>20242618</v>
+      </c>
+      <c r="E357" s="8" t="s">
+        <v>908</v>
+      </c>
+      <c r="F357" s="8">
+        <v>3</v>
+      </c>
+      <c r="G357" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="H357" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I357" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J357" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="K357" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L357" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M357" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N357" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O357" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P357" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q357" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R357" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S357" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T357" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="U357" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V357" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W357" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X357" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y357" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z357" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA357" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB357" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC357" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD357" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="358" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A358" s="4">
+        <v>45571.644409791668</v>
+      </c>
+      <c r="B358" s="5" t="s">
+        <v>909</v>
+      </c>
+      <c r="C358" s="5" t="s">
+        <v>910</v>
+      </c>
+      <c r="D358" s="5">
+        <v>20201031</v>
+      </c>
+      <c r="E358" s="5" t="s">
+        <v>911</v>
+      </c>
+      <c r="F358" s="5">
+        <v>3</v>
+      </c>
+      <c r="G358" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="H358" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I358" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="J358" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="K358" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L358" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="M358" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="N358" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O358" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P358" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q358" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R358" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="S358" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T358" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U358" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="V358" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="W358" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="X358" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y358" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z358" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA358" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB358" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC358" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="AD358" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="359" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A359" s="7">
+        <v>45571.64736855324</v>
+      </c>
+      <c r="B359" s="8" t="s">
+        <v>912</v>
+      </c>
+      <c r="C359" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D359" s="8">
+        <v>20242101</v>
+      </c>
+      <c r="E359" s="8" t="s">
+        <v>913</v>
+      </c>
+      <c r="F359" s="8">
+        <v>3</v>
+      </c>
+      <c r="G359" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H359" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I359" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J359" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K359" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L359" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M359" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N359" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O359" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P359" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q359" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R359" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S359" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T359" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="U359" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V359" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W359" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X359" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y359" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z359" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA359" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB359" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC359" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD359" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="360" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A360" s="4">
+        <v>45571.658410891207</v>
+      </c>
+      <c r="B360" s="5" t="s">
+        <v>914</v>
+      </c>
+      <c r="C360" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D360" s="5">
+        <v>20203537</v>
+      </c>
+      <c r="E360" s="5" t="s">
+        <v>915</v>
+      </c>
+      <c r="F360" s="5">
+        <v>3</v>
+      </c>
+      <c r="G360" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H360" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I360" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J360" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K360" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L360" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M360" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="N360" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O360" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P360" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q360" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R360" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S360" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T360" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U360" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V360" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="W360" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X360" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y360" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z360" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA360" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB360" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC360" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD360" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="361" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A361" s="7">
+        <v>45571.663042418979</v>
+      </c>
+      <c r="B361" s="8" t="s">
+        <v>916</v>
+      </c>
+      <c r="C361" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="D361" s="8">
+        <v>20242981</v>
+      </c>
+      <c r="E361" s="8" t="s">
+        <v>917</v>
+      </c>
+      <c r="F361" s="8">
+        <v>3</v>
+      </c>
+      <c r="G361" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H361" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I361" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J361" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K361" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L361" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M361" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N361" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O361" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P361" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q361" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R361" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S361" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T361" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U361" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V361" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W361" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X361" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y361" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z361" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA361" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB361" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC361" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD361" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="362" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A362" s="4">
+        <v>45571.681314398149</v>
+      </c>
+      <c r="B362" s="5" t="s">
+        <v>918</v>
+      </c>
+      <c r="C362" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="D362" s="5">
+        <v>20191240</v>
+      </c>
+      <c r="E362" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="F362" s="5">
+        <v>3</v>
+      </c>
+      <c r="G362" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H362" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I362" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J362" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K362" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L362" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M362" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N362" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O362" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P362" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q362" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R362" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S362" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T362" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U362" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V362" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W362" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X362" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y362" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z362" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA362" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB362" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC362" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD362" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="363" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A363" s="7">
+        <v>45571.686560682865</v>
+      </c>
+      <c r="B363" s="8" t="s">
+        <v>920</v>
+      </c>
+      <c r="C363" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D363" s="8">
+        <v>20192717</v>
+      </c>
+      <c r="E363" s="8" t="s">
+        <v>921</v>
+      </c>
+      <c r="F363" s="8">
+        <v>3</v>
+      </c>
+      <c r="G363" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H363" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I363" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J363" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K363" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L363" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M363" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N363" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O363" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P363" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q363" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R363" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S363" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T363" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="U363" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V363" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W363" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X363" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y363" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z363" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA363" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB363" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC363" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD363" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="364" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A364" s="4">
+        <v>45571.694631087958</v>
+      </c>
+      <c r="B364" s="5" t="s">
+        <v>922</v>
+      </c>
+      <c r="C364" s="5" t="s">
+        <v>923</v>
+      </c>
+      <c r="D364" s="5">
+        <v>20193341</v>
+      </c>
+      <c r="E364" s="5" t="s">
+        <v>924</v>
+      </c>
+      <c r="F364" s="5">
+        <v>3</v>
+      </c>
+      <c r="G364" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H364" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I364" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J364" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="K364" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L364" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="M364" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="N364" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O364" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="P364" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q364" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R364" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="S364" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="T364" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U364" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="V364" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="W364" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="X364" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y364" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z364" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA364" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB364" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC364" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD364" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="365" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A365" s="7">
+        <v>45571.704429872683</v>
+      </c>
+      <c r="B365" s="8" t="s">
+        <v>925</v>
+      </c>
+      <c r="C365" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D365" s="8">
+        <v>20214143</v>
+      </c>
+      <c r="E365" s="8" t="s">
+        <v>926</v>
+      </c>
+      <c r="F365" s="8">
+        <v>3</v>
+      </c>
+      <c r="G365" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H365" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I365" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J365" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="K365" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L365" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M365" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N365" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O365" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P365" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q365" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R365" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="S365" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T365" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="U365" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V365" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W365" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X365" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y365" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z365" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA365" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB365" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC365" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD365" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="366" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A366" s="4">
+        <v>45571.712937037039</v>
+      </c>
+      <c r="B366" s="5" t="s">
+        <v>927</v>
+      </c>
+      <c r="C366" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="D366" s="5">
+        <v>20233412</v>
+      </c>
+      <c r="E366" s="5" t="s">
+        <v>928</v>
+      </c>
+      <c r="F366" s="5">
+        <v>3</v>
+      </c>
+      <c r="G366" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H366" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I366" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J366" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K366" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L366" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M366" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N366" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O366" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P366" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q366" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R366" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S366" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T366" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U366" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V366" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W366" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X366" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y366" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z366" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA366" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB366" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC366" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD366" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="367" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A367" s="7">
+        <v>45571.718232719912</v>
+      </c>
+      <c r="B367" s="8" t="s">
+        <v>929</v>
+      </c>
+      <c r="C367" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D367" s="8">
+        <v>20231622</v>
+      </c>
+      <c r="E367" s="8" t="s">
+        <v>930</v>
+      </c>
+      <c r="F367" s="8">
+        <v>3</v>
+      </c>
+      <c r="G367" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H367" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I367" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J367" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K367" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L367" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M367" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N367" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O367" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P367" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q367" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R367" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S367" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T367" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U367" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V367" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W367" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X367" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y367" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z367" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA367" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB367" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC367" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD367" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="368" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A368" s="4">
+        <v>45571.720994641204</v>
+      </c>
+      <c r="B368" s="5" t="s">
+        <v>931</v>
+      </c>
+      <c r="C368" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D368" s="5">
+        <v>20192721</v>
+      </c>
+      <c r="E368" s="5" t="s">
+        <v>932</v>
+      </c>
+      <c r="F368" s="5">
+        <v>3</v>
+      </c>
+      <c r="G368" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H368" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I368" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J368" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K368" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L368" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M368" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N368" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O368" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P368" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q368" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R368" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S368" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T368" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U368" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V368" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W368" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X368" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y368" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z368" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA368" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB368" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC368" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD368" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="369" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A369" s="7">
+        <v>45571.721850393515</v>
+      </c>
+      <c r="B369" s="8" t="s">
+        <v>933</v>
+      </c>
+      <c r="C369" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D369" s="8">
+        <v>20227073</v>
+      </c>
+      <c r="E369" s="8" t="s">
+        <v>934</v>
+      </c>
+      <c r="F369" s="8">
+        <v>3</v>
+      </c>
+      <c r="G369" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H369" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I369" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J369" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K369" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L369" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M369" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N369" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O369" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="P369" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q369" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R369" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S369" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T369" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U369" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V369" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W369" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X369" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y369" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z369" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA369" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB369" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC369" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD369" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="370" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A370" s="16">
+        <v>45571.740967129634</v>
+      </c>
+      <c r="B370" s="17" t="s">
+        <v>935</v>
+      </c>
+      <c r="C370" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D370" s="17">
+        <v>20243803</v>
+      </c>
+      <c r="E370" s="17" t="s">
+        <v>936</v>
+      </c>
+      <c r="F370" s="17">
+        <v>3</v>
+      </c>
+      <c r="G370" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H370" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="I370" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="J370" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="K370" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="L370" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="M370" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="N370" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="O370" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="P370" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q370" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="R370" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="S370" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="T370" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="U370" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="V370" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="W370" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="X370" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y370" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z370" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA370" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB370" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC370" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD370" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
literacy, 240930 modified 11
</commit_message>
<xml_diff>
--- a/R/data/literacy_240930.xlsx
+++ b/R/data/literacy_240930.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2B10D0-F7A9-A04B-96BD-4E27A478BE06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F76BFC-01EE-1048-9393-7FE3032644CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50400" yWindow="1360" windowWidth="44800" windowHeight="24700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9993" uniqueCount="937">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11208" uniqueCount="1028">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -2831,6 +2831,279 @@
   </si>
   <si>
     <t>권하늘</t>
+  </si>
+  <si>
+    <t>bcy1976@naver.com</t>
+  </si>
+  <si>
+    <t>변치윤</t>
+  </si>
+  <si>
+    <t>youmakein@gmail.com</t>
+  </si>
+  <si>
+    <t>seon93804@gmail.com</t>
+  </si>
+  <si>
+    <t>김인선</t>
+  </si>
+  <si>
+    <t>kmu2916@naver.com</t>
+  </si>
+  <si>
+    <t>강민욱</t>
+  </si>
+  <si>
+    <t>ghkdxo2003@gmail.com</t>
+  </si>
+  <si>
+    <t>황이준</t>
+  </si>
+  <si>
+    <t>minuhwang16@gmail.com</t>
+  </si>
+  <si>
+    <t>황민우</t>
+  </si>
+  <si>
+    <t>syb00syb00@naver.com</t>
+  </si>
+  <si>
+    <t>신유비</t>
+  </si>
+  <si>
+    <t>leejs7807@gmail.com</t>
+  </si>
+  <si>
+    <t>이종선</t>
+  </si>
+  <si>
+    <t>namryumin@gmail.com</t>
+  </si>
+  <si>
+    <t>남류민</t>
+  </si>
+  <si>
+    <t>goemf100@naver.com</t>
+  </si>
+  <si>
+    <t>jeongminyoung13@gmail.com</t>
+  </si>
+  <si>
+    <t>정민영</t>
+  </si>
+  <si>
+    <t>chsmdfur123@naver.com</t>
+  </si>
+  <si>
+    <t>금융재무</t>
+  </si>
+  <si>
+    <t>이한얼</t>
+  </si>
+  <si>
+    <t>na1448@naver.com</t>
+  </si>
+  <si>
+    <t>강나현</t>
+  </si>
+  <si>
+    <t>tonykim0703@gmail.com</t>
+  </si>
+  <si>
+    <t>김주엽</t>
+  </si>
+  <si>
+    <t>ran0753@gmail.com</t>
+  </si>
+  <si>
+    <t>김태란</t>
+  </si>
+  <si>
+    <t>cjfghksznszns1100119@naver.com</t>
+  </si>
+  <si>
+    <t>유철환</t>
+  </si>
+  <si>
+    <t>dayae6762@naver.com</t>
+  </si>
+  <si>
+    <t>장다예</t>
+  </si>
+  <si>
+    <t>chiyoon12@gmail.com</t>
+  </si>
+  <si>
+    <t>김치윤</t>
+  </si>
+  <si>
+    <t>qortjdus27@naver.com</t>
+  </si>
+  <si>
+    <t>백서연</t>
+  </si>
+  <si>
+    <t>jina20050429@gmail.com</t>
+  </si>
+  <si>
+    <t>이진아</t>
+  </si>
+  <si>
+    <t>dawn2368@gmail.com</t>
+  </si>
+  <si>
+    <t>허다운</t>
+  </si>
+  <si>
+    <t>chlwnstn777@naver.com</t>
+  </si>
+  <si>
+    <t>빅데이터 전공</t>
+  </si>
+  <si>
+    <t>최준수</t>
+  </si>
+  <si>
+    <t>lyn392392@naver.com</t>
+  </si>
+  <si>
+    <t>이유나</t>
+  </si>
+  <si>
+    <t>jsh050906@naver.com</t>
+  </si>
+  <si>
+    <t>정송희</t>
+  </si>
+  <si>
+    <t>asrud8755@naver.com</t>
+  </si>
+  <si>
+    <t>jsk991012@naver.com</t>
+  </si>
+  <si>
+    <t>김준서</t>
+  </si>
+  <si>
+    <t>jdragon0151@gmail.com</t>
+  </si>
+  <si>
+    <t>신준용</t>
+  </si>
+  <si>
+    <t>jin0321558@gmail.com</t>
+  </si>
+  <si>
+    <t>전시연</t>
+  </si>
+  <si>
+    <t>5tmddk@naver.com</t>
+  </si>
+  <si>
+    <t>최승아</t>
+  </si>
+  <si>
+    <t>giyongi37@gmail.com</t>
+  </si>
+  <si>
+    <t>이기용</t>
+  </si>
+  <si>
+    <t>77sunhwa@gmail.com</t>
+  </si>
+  <si>
+    <t>박선화</t>
+  </si>
+  <si>
+    <t>ss0001234@naver.com</t>
+  </si>
+  <si>
+    <t>김세은</t>
+  </si>
+  <si>
+    <t>rabbit1657@gmail.com</t>
+  </si>
+  <si>
+    <t>이예원</t>
+  </si>
+  <si>
+    <t>bsgtopriner0@gmail.com</t>
+  </si>
+  <si>
+    <t>최윤혁</t>
+  </si>
+  <si>
+    <t>ism050204@naver.com</t>
+  </si>
+  <si>
+    <t>leedug87@gmail.com</t>
+  </si>
+  <si>
+    <t>이두현</t>
+  </si>
+  <si>
+    <t>parkjinseo23@naver.com</t>
+  </si>
+  <si>
+    <t>his86814189@gmail.com</t>
+  </si>
+  <si>
+    <t>황인성</t>
+  </si>
+  <si>
+    <t>eseses0827@naver.com</t>
+  </si>
+  <si>
+    <t>강은서</t>
+  </si>
+  <si>
+    <t>lucy37lucy37lucy37@naver.com</t>
+  </si>
+  <si>
+    <t>이은지</t>
+  </si>
+  <si>
+    <t>seungye04@naver.com</t>
+  </si>
+  <si>
+    <t>언론방송융합미디어</t>
+  </si>
+  <si>
+    <t>정승예</t>
+  </si>
+  <si>
+    <t>zzun1414@naver.com</t>
+  </si>
+  <si>
+    <t>반도체·디스플레이스쿨</t>
+  </si>
+  <si>
+    <t>황준영</t>
+  </si>
+  <si>
+    <t>yeonh990@naver.com</t>
+  </si>
+  <si>
+    <t>언어병리학전공</t>
+  </si>
+  <si>
+    <t>박현아</t>
+  </si>
+  <si>
+    <t>orientfun@gmail.com</t>
+  </si>
+  <si>
+    <t>소프트웨어학</t>
+  </si>
+  <si>
+    <t>이동화</t>
+  </si>
+  <si>
+    <t>KMS050915@NAVER.COM</t>
+  </si>
+  <si>
+    <t>강명수</t>
   </si>
 </sst>
 </file>
@@ -3245,7 +3518,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:AD370">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:AD415">
   <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -3483,11 +3756,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD370"/>
+  <dimension ref="A1:AD415"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A327" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F382" sqref="F382"/>
+      <pane ySplit="1" topLeftCell="A354" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D418" sqref="D418"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -37560,6 +37833,4146 @@
         <v>56</v>
       </c>
     </row>
+    <row r="371" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A371" s="7">
+        <v>45571.748642245366</v>
+      </c>
+      <c r="B371" s="8" t="s">
+        <v>937</v>
+      </c>
+      <c r="C371" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="D371" s="8">
+        <v>20235180</v>
+      </c>
+      <c r="E371" s="8" t="s">
+        <v>938</v>
+      </c>
+      <c r="F371" s="8">
+        <v>3</v>
+      </c>
+      <c r="G371" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H371" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I371" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J371" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K371" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="L371" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M371" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="N371" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O371" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P371" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q371" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R371" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S371" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T371" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="U371" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V371" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W371" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X371" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y371" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z371" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA371" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB371" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC371" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD371" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="372" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A372" s="4">
+        <v>45571.750233275467</v>
+      </c>
+      <c r="B372" s="5" t="s">
+        <v>939</v>
+      </c>
+      <c r="C372" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D372" s="5">
+        <v>20241106</v>
+      </c>
+      <c r="E372" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="F372" s="5">
+        <v>3</v>
+      </c>
+      <c r="G372" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H372" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I372" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J372" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K372" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L372" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M372" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N372" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O372" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P372" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q372" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R372" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S372" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T372" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="U372" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V372" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W372" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X372" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y372" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z372" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA372" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB372" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC372" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD372" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="373" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A373" s="7">
+        <v>45571.751078634261</v>
+      </c>
+      <c r="B373" s="8" t="s">
+        <v>940</v>
+      </c>
+      <c r="C373" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="D373" s="8">
+        <v>20221209</v>
+      </c>
+      <c r="E373" s="8" t="s">
+        <v>941</v>
+      </c>
+      <c r="F373" s="8">
+        <v>3</v>
+      </c>
+      <c r="G373" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H373" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I373" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J373" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K373" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L373" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M373" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N373" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O373" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P373" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q373" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R373" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S373" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T373" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="U373" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V373" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="W373" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X373" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y373" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z373" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA373" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB373" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC373" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="AD373" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="374" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A374" s="4">
+        <v>45571.760614826388</v>
+      </c>
+      <c r="B374" s="5" t="s">
+        <v>942</v>
+      </c>
+      <c r="C374" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D374" s="5">
+        <v>20222902</v>
+      </c>
+      <c r="E374" s="5" t="s">
+        <v>943</v>
+      </c>
+      <c r="F374" s="5">
+        <v>3</v>
+      </c>
+      <c r="G374" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H374" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I374" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J374" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K374" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L374" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M374" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N374" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O374" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P374" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q374" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R374" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S374" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T374" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U374" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V374" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W374" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X374" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y374" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z374" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA374" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB374" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC374" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD374" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="375" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A375" s="7">
+        <v>45571.766540798606</v>
+      </c>
+      <c r="B375" s="8" t="s">
+        <v>944</v>
+      </c>
+      <c r="C375" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="D375" s="8">
+        <v>20231733</v>
+      </c>
+      <c r="E375" s="8" t="s">
+        <v>945</v>
+      </c>
+      <c r="F375" s="8">
+        <v>3</v>
+      </c>
+      <c r="G375" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H375" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I375" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J375" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K375" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="L375" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M375" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N375" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O375" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P375" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q375" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R375" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S375" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T375" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U375" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="V375" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W375" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X375" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y375" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z375" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA375" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB375" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC375" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD375" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="376" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A376" s="4">
+        <v>45571.785545694445</v>
+      </c>
+      <c r="B376" s="5" t="s">
+        <v>946</v>
+      </c>
+      <c r="C376" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D376" s="5">
+        <v>20243967</v>
+      </c>
+      <c r="E376" s="5" t="s">
+        <v>947</v>
+      </c>
+      <c r="F376" s="5">
+        <v>3</v>
+      </c>
+      <c r="G376" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H376" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I376" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J376" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K376" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L376" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M376" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="N376" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O376" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P376" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q376" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R376" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S376" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="T376" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U376" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="V376" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W376" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="X376" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y376" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z376" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA376" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB376" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC376" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD376" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="377" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A377" s="7">
+        <v>45571.786135671297</v>
+      </c>
+      <c r="B377" s="8" t="s">
+        <v>948</v>
+      </c>
+      <c r="C377" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D377" s="8">
+        <v>20234128</v>
+      </c>
+      <c r="E377" s="8" t="s">
+        <v>949</v>
+      </c>
+      <c r="F377" s="8">
+        <v>3</v>
+      </c>
+      <c r="G377" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="H377" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I377" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J377" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="K377" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="L377" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="M377" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N377" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O377" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="P377" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q377" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R377" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="S377" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T377" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U377" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="V377" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W377" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="X377" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y377" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z377" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA377" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB377" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC377" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD377" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="378" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A378" s="4">
+        <v>45571.812119953705</v>
+      </c>
+      <c r="B378" s="5" t="s">
+        <v>950</v>
+      </c>
+      <c r="C378" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="D378" s="5">
+        <v>20223249</v>
+      </c>
+      <c r="E378" s="5" t="s">
+        <v>951</v>
+      </c>
+      <c r="F378" s="5">
+        <v>3</v>
+      </c>
+      <c r="G378" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H378" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I378" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J378" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K378" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L378" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M378" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="N378" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O378" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="P378" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q378" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R378" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S378" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T378" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="U378" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V378" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W378" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X378" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y378" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z378" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AA378" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB378" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC378" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD378" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="379" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A379" s="7">
+        <v>45571.824242534727</v>
+      </c>
+      <c r="B379" s="8" t="s">
+        <v>952</v>
+      </c>
+      <c r="C379" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D379" s="8">
+        <v>20245154</v>
+      </c>
+      <c r="E379" s="8" t="s">
+        <v>953</v>
+      </c>
+      <c r="F379" s="8">
+        <v>3</v>
+      </c>
+      <c r="G379" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H379" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I379" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J379" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K379" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L379" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M379" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N379" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O379" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P379" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q379" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R379" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S379" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T379" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="U379" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V379" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W379" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X379" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y379" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z379" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA379" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB379" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC379" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD379" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="380" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A380" s="4">
+        <v>45571.827457326392</v>
+      </c>
+      <c r="B380" s="5" t="s">
+        <v>954</v>
+      </c>
+      <c r="C380" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D380" s="5">
+        <v>20222709</v>
+      </c>
+      <c r="E380" s="5" t="s">
+        <v>520</v>
+      </c>
+      <c r="F380" s="5">
+        <v>3</v>
+      </c>
+      <c r="G380" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H380" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I380" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J380" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K380" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L380" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M380" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N380" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O380" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P380" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q380" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R380" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S380" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T380" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="U380" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="V380" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W380" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X380" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y380" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z380" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA380" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB380" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC380" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD380" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="381" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A381" s="7">
+        <v>45571.834519328702</v>
+      </c>
+      <c r="B381" s="8" t="s">
+        <v>955</v>
+      </c>
+      <c r="C381" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D381" s="8">
+        <v>20246281</v>
+      </c>
+      <c r="E381" s="8" t="s">
+        <v>956</v>
+      </c>
+      <c r="F381" s="8">
+        <v>3</v>
+      </c>
+      <c r="G381" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H381" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I381" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J381" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K381" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L381" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M381" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N381" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O381" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P381" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q381" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R381" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S381" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T381" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U381" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V381" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W381" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X381" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y381" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z381" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA381" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB381" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC381" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD381" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="382" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A382" s="4">
+        <v>45571.835515370374</v>
+      </c>
+      <c r="B382" s="5" t="s">
+        <v>957</v>
+      </c>
+      <c r="C382" s="5" t="s">
+        <v>958</v>
+      </c>
+      <c r="D382" s="5">
+        <v>20203026</v>
+      </c>
+      <c r="E382" s="5" t="s">
+        <v>959</v>
+      </c>
+      <c r="F382" s="5">
+        <v>3</v>
+      </c>
+      <c r="G382" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H382" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I382" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J382" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K382" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L382" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M382" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N382" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O382" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P382" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q382" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R382" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S382" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T382" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U382" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V382" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W382" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X382" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y382" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z382" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA382" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB382" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC382" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD382" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="383" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A383" s="7">
+        <v>45571.837896921294</v>
+      </c>
+      <c r="B383" s="8" t="s">
+        <v>960</v>
+      </c>
+      <c r="C383" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="D383" s="8">
+        <v>20243601</v>
+      </c>
+      <c r="E383" s="8" t="s">
+        <v>961</v>
+      </c>
+      <c r="F383" s="8">
+        <v>3</v>
+      </c>
+      <c r="G383" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H383" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I383" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J383" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K383" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L383" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M383" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N383" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O383" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P383" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q383" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R383" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="S383" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="T383" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U383" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V383" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="W383" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="X383" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y383" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z383" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA383" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB383" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC383" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD383" s="9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="384" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A384" s="4">
+        <v>45571.838250011569</v>
+      </c>
+      <c r="B384" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="C384" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D384" s="5">
+        <v>20213709</v>
+      </c>
+      <c r="E384" s="5" t="s">
+        <v>963</v>
+      </c>
+      <c r="F384" s="5">
+        <v>3</v>
+      </c>
+      <c r="G384" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H384" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I384" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J384" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K384" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L384" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M384" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N384" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O384" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P384" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q384" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R384" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S384" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T384" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U384" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V384" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W384" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X384" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y384" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z384" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA384" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB384" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC384" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD384" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="385" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A385" s="7">
+        <v>45571.841559525463</v>
+      </c>
+      <c r="B385" s="8" t="s">
+        <v>964</v>
+      </c>
+      <c r="C385" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="D385" s="8">
+        <v>20243615</v>
+      </c>
+      <c r="E385" s="8" t="s">
+        <v>965</v>
+      </c>
+      <c r="F385" s="8">
+        <v>3</v>
+      </c>
+      <c r="G385" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="H385" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I385" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J385" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="K385" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="L385" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="M385" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N385" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O385" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P385" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q385" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R385" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S385" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T385" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="U385" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V385" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W385" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X385" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y385" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z385" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA385" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB385" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC385" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD385" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="386" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A386" s="4">
+        <v>45571.841954074072</v>
+      </c>
+      <c r="B386" s="5" t="s">
+        <v>966</v>
+      </c>
+      <c r="C386" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D386" s="5">
+        <v>20243829</v>
+      </c>
+      <c r="E386" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="F386" s="5">
+        <v>3</v>
+      </c>
+      <c r="G386" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H386" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I386" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J386" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K386" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L386" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M386" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N386" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O386" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P386" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q386" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R386" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S386" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T386" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U386" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V386" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W386" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X386" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y386" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z386" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA386" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB386" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC386" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD386" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="387" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A387" s="7">
+        <v>45571.846048854168</v>
+      </c>
+      <c r="B387" s="8" t="s">
+        <v>968</v>
+      </c>
+      <c r="C387" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D387" s="8">
+        <v>20241081</v>
+      </c>
+      <c r="E387" s="8" t="s">
+        <v>969</v>
+      </c>
+      <c r="F387" s="8">
+        <v>3</v>
+      </c>
+      <c r="G387" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H387" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I387" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J387" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K387" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L387" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M387" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="N387" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O387" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P387" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q387" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R387" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S387" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T387" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U387" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V387" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W387" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X387" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y387" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z387" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA387" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB387" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC387" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD387" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="388" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A388" s="4">
+        <v>45571.847320312503</v>
+      </c>
+      <c r="B388" s="5" t="s">
+        <v>970</v>
+      </c>
+      <c r="C388" s="5" t="s">
+        <v>762</v>
+      </c>
+      <c r="D388" s="5">
+        <v>20232938</v>
+      </c>
+      <c r="E388" s="5" t="s">
+        <v>971</v>
+      </c>
+      <c r="F388" s="5">
+        <v>3</v>
+      </c>
+      <c r="G388" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H388" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I388" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J388" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K388" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L388" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M388" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="N388" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O388" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P388" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q388" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R388" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S388" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T388" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U388" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V388" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W388" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X388" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y388" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z388" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA388" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB388" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC388" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD388" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="389" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A389" s="7">
+        <v>45571.856485162032</v>
+      </c>
+      <c r="B389" s="8" t="s">
+        <v>972</v>
+      </c>
+      <c r="C389" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="D389" s="8">
+        <v>20242971</v>
+      </c>
+      <c r="E389" s="8" t="s">
+        <v>973</v>
+      </c>
+      <c r="F389" s="8">
+        <v>3</v>
+      </c>
+      <c r="G389" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H389" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I389" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J389" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K389" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L389" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M389" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N389" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O389" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P389" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q389" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R389" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S389" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T389" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U389" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V389" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W389" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X389" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y389" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z389" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA389" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB389" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC389" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD389" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="390" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A390" s="4">
+        <v>45571.860138414355</v>
+      </c>
+      <c r="B390" s="5" t="s">
+        <v>974</v>
+      </c>
+      <c r="C390" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D390" s="5">
+        <v>20243731</v>
+      </c>
+      <c r="E390" s="5" t="s">
+        <v>975</v>
+      </c>
+      <c r="F390" s="5">
+        <v>3</v>
+      </c>
+      <c r="G390" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="H390" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I390" s="5" t="s">
+        <v>760</v>
+      </c>
+      <c r="J390" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K390" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L390" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="M390" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="N390" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O390" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P390" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q390" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R390" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S390" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="T390" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U390" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="V390" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W390" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="X390" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y390" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z390" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA390" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB390" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC390" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD390" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="391" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A391" s="7">
+        <v>45571.874193807875</v>
+      </c>
+      <c r="B391" s="8" t="s">
+        <v>976</v>
+      </c>
+      <c r="C391" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D391" s="8">
+        <v>20197126</v>
+      </c>
+      <c r="E391" s="8" t="s">
+        <v>977</v>
+      </c>
+      <c r="F391" s="8">
+        <v>3</v>
+      </c>
+      <c r="G391" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H391" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I391" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J391" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K391" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L391" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M391" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N391" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O391" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P391" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q391" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R391" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S391" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T391" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U391" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V391" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W391" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X391" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y391" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z391" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA391" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB391" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC391" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD391" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="392" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A392" s="4">
+        <v>45571.875075462958</v>
+      </c>
+      <c r="B392" s="5" t="s">
+        <v>978</v>
+      </c>
+      <c r="C392" s="5" t="s">
+        <v>979</v>
+      </c>
+      <c r="D392" s="5">
+        <v>20193844</v>
+      </c>
+      <c r="E392" s="5" t="s">
+        <v>980</v>
+      </c>
+      <c r="F392" s="5">
+        <v>3</v>
+      </c>
+      <c r="G392" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H392" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I392" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J392" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K392" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L392" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M392" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N392" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O392" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P392" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q392" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R392" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S392" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T392" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U392" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V392" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W392" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X392" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y392" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z392" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA392" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB392" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC392" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD392" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="393" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A393" s="7">
+        <v>45571.876548912041</v>
+      </c>
+      <c r="B393" s="8" t="s">
+        <v>981</v>
+      </c>
+      <c r="C393" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="D393" s="8">
+        <v>20243007</v>
+      </c>
+      <c r="E393" s="8" t="s">
+        <v>982</v>
+      </c>
+      <c r="F393" s="8">
+        <v>3</v>
+      </c>
+      <c r="G393" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H393" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I393" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J393" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K393" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L393" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M393" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N393" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O393" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P393" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q393" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R393" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S393" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T393" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U393" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V393" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W393" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X393" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y393" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z393" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA393" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB393" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC393" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD393" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="394" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A394" s="4">
+        <v>45571.881279131943</v>
+      </c>
+      <c r="B394" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="C394" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="D394" s="5">
+        <v>20243032</v>
+      </c>
+      <c r="E394" s="5" t="s">
+        <v>984</v>
+      </c>
+      <c r="F394" s="5">
+        <v>3</v>
+      </c>
+      <c r="G394" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H394" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I394" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J394" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K394" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L394" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M394" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N394" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O394" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P394" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q394" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R394" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S394" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="T394" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U394" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V394" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W394" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X394" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y394" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z394" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA394" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB394" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC394" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD394" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="395" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A395" s="7">
+        <v>45571.890264305555</v>
+      </c>
+      <c r="B395" s="8" t="s">
+        <v>985</v>
+      </c>
+      <c r="C395" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="D395" s="8">
+        <v>20222606</v>
+      </c>
+      <c r="E395" s="8" t="s">
+        <v>498</v>
+      </c>
+      <c r="F395" s="8">
+        <v>3</v>
+      </c>
+      <c r="G395" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H395" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I395" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J395" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K395" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="L395" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M395" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N395" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O395" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P395" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q395" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R395" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S395" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T395" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="U395" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V395" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W395" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X395" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y395" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z395" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA395" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB395" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC395" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD395" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="396" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A396" s="16">
+        <v>45571.907073599534</v>
+      </c>
+      <c r="B396" s="17" t="s">
+        <v>986</v>
+      </c>
+      <c r="C396" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="D396" s="17">
+        <v>20182519</v>
+      </c>
+      <c r="E396" s="17" t="s">
+        <v>987</v>
+      </c>
+      <c r="F396" s="17">
+        <v>3</v>
+      </c>
+      <c r="G396" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H396" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="I396" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="J396" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="K396" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="L396" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="M396" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="N396" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="O396" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="P396" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q396" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="R396" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="S396" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="T396" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="U396" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="V396" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="W396" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="X396" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y396" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z396" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA396" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB396" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC396" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD396" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="397" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A397" s="7">
+        <v>45571.914914212961</v>
+      </c>
+      <c r="B397" s="8" t="s">
+        <v>988</v>
+      </c>
+      <c r="C397" s="8" t="s">
+        <v>485</v>
+      </c>
+      <c r="D397" s="8">
+        <v>20205195</v>
+      </c>
+      <c r="E397" s="8" t="s">
+        <v>989</v>
+      </c>
+      <c r="F397" s="8">
+        <v>3</v>
+      </c>
+      <c r="G397" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H397" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I397" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J397" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K397" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L397" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M397" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N397" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O397" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P397" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q397" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R397" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S397" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T397" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="U397" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V397" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W397" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X397" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y397" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z397" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA397" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB397" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC397" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD397" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="398" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A398" s="4">
+        <v>45571.91700887731</v>
+      </c>
+      <c r="B398" s="5" t="s">
+        <v>990</v>
+      </c>
+      <c r="C398" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="D398" s="5">
+        <v>20246932</v>
+      </c>
+      <c r="E398" s="5" t="s">
+        <v>991</v>
+      </c>
+      <c r="F398" s="5">
+        <v>3</v>
+      </c>
+      <c r="G398" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H398" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I398" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J398" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K398" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L398" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M398" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N398" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O398" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="P398" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q398" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="R398" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="S398" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="T398" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="U398" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="V398" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="W398" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="X398" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y398" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z398" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA398" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB398" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC398" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD398" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="399" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A399" s="7">
+        <v>45571.920124259261</v>
+      </c>
+      <c r="B399" s="8" t="s">
+        <v>992</v>
+      </c>
+      <c r="C399" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="D399" s="8">
+        <v>20192634</v>
+      </c>
+      <c r="E399" s="8" t="s">
+        <v>993</v>
+      </c>
+      <c r="F399" s="8">
+        <v>3</v>
+      </c>
+      <c r="G399" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H399" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I399" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J399" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K399" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L399" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M399" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N399" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O399" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P399" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q399" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R399" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S399" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T399" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="U399" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V399" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W399" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X399" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y399" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z399" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA399" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB399" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC399" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="AD399" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="400" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A400" s="4">
+        <v>45571.927768368056</v>
+      </c>
+      <c r="B400" s="5" t="s">
+        <v>994</v>
+      </c>
+      <c r="C400" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="D400" s="5">
+        <v>20215199</v>
+      </c>
+      <c r="E400" s="5" t="s">
+        <v>995</v>
+      </c>
+      <c r="F400" s="5">
+        <v>3</v>
+      </c>
+      <c r="G400" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="H400" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I400" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J400" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="K400" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L400" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="M400" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="N400" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O400" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="P400" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q400" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R400" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="S400" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="T400" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U400" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="V400" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="W400" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="X400" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y400" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z400" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AA400" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB400" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC400" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD400" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="401" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A401" s="7">
+        <v>45571.938911736113</v>
+      </c>
+      <c r="B401" s="8" t="s">
+        <v>996</v>
+      </c>
+      <c r="C401" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="D401" s="8">
+        <v>20242956</v>
+      </c>
+      <c r="E401" s="8" t="s">
+        <v>997</v>
+      </c>
+      <c r="F401" s="8">
+        <v>3</v>
+      </c>
+      <c r="G401" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H401" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I401" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J401" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K401" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L401" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M401" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N401" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O401" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P401" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q401" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R401" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S401" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T401" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U401" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V401" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W401" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X401" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y401" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z401" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA401" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB401" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC401" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD401" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="402" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A402" s="4">
+        <v>45571.949017789353</v>
+      </c>
+      <c r="B402" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="C402" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D402" s="5">
+        <v>20203211</v>
+      </c>
+      <c r="E402" s="5" t="s">
+        <v>999</v>
+      </c>
+      <c r="F402" s="5">
+        <v>3</v>
+      </c>
+      <c r="G402" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H402" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I402" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J402" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K402" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L402" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M402" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N402" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O402" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P402" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q402" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R402" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S402" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T402" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U402" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="V402" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W402" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X402" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y402" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z402" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA402" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB402" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC402" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD402" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="403" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A403" s="7">
+        <v>45571.952060925927</v>
+      </c>
+      <c r="B403" s="8" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C403" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D403" s="8">
+        <v>20243939</v>
+      </c>
+      <c r="E403" s="8" t="s">
+        <v>1001</v>
+      </c>
+      <c r="F403" s="8">
+        <v>3</v>
+      </c>
+      <c r="G403" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H403" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I403" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J403" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K403" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L403" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M403" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N403" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O403" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P403" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q403" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R403" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S403" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T403" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U403" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V403" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W403" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X403" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y403" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z403" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA403" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB403" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC403" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD403" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="404" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A404" s="4">
+        <v>45571.954713206018</v>
+      </c>
+      <c r="B404" s="5" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C404" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="D404" s="5">
+        <v>20242636</v>
+      </c>
+      <c r="E404" s="5" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F404" s="5">
+        <v>3</v>
+      </c>
+      <c r="G404" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H404" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I404" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J404" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K404" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L404" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M404" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N404" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O404" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P404" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q404" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R404" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S404" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T404" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U404" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V404" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W404" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X404" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y404" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z404" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA404" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB404" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC404" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD404" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="405" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A405" s="7">
+        <v>45571.961079247689</v>
+      </c>
+      <c r="B405" s="8" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C405" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D405" s="8">
+        <v>20243001</v>
+      </c>
+      <c r="E405" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="F405" s="8">
+        <v>3</v>
+      </c>
+      <c r="G405" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H405" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I405" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J405" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K405" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L405" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M405" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N405" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O405" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P405" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q405" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R405" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S405" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T405" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U405" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V405" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W405" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X405" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y405" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z405" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA405" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB405" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC405" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD405" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="406" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A406" s="4">
+        <v>45571.962926400462</v>
+      </c>
+      <c r="B406" s="5" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C406" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D406" s="5">
+        <v>20231623</v>
+      </c>
+      <c r="E406" s="5" t="s">
+        <v>1006</v>
+      </c>
+      <c r="F406" s="5">
+        <v>3</v>
+      </c>
+      <c r="G406" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H406" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I406" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J406" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="K406" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L406" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M406" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N406" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O406" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P406" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q406" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R406" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S406" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T406" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U406" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V406" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W406" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X406" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y406" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z406" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA406" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB406" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC406" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD406" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="407" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A407" s="7">
+        <v>45571.964145891208</v>
+      </c>
+      <c r="B407" s="8" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C407" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D407" s="8">
+        <v>20242824</v>
+      </c>
+      <c r="E407" s="8" t="s">
+        <v>875</v>
+      </c>
+      <c r="F407" s="8">
+        <v>3</v>
+      </c>
+      <c r="G407" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H407" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I407" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J407" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K407" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L407" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="M407" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N407" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="O407" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="P407" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q407" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="R407" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="S407" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T407" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="U407" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="V407" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W407" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="X407" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="Y407" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z407" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA407" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB407" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="AC407" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD407" s="9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="408" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A408" s="4">
+        <v>45571.965810185182</v>
+      </c>
+      <c r="B408" s="5" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C408" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="D408" s="5">
+        <v>20246942</v>
+      </c>
+      <c r="E408" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F408" s="5">
+        <v>3</v>
+      </c>
+      <c r="G408" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H408" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I408" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J408" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="K408" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="L408" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M408" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N408" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O408" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P408" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q408" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R408" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S408" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T408" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U408" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V408" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W408" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X408" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y408" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z408" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA408" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB408" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC408" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD408" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="409" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A409" s="7">
+        <v>45571.978636504631</v>
+      </c>
+      <c r="B409" s="8" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C409" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="D409" s="8">
+        <v>20241503</v>
+      </c>
+      <c r="E409" s="8" t="s">
+        <v>1011</v>
+      </c>
+      <c r="F409" s="8">
+        <v>3</v>
+      </c>
+      <c r="G409" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H409" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I409" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J409" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K409" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="L409" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M409" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N409" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O409" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P409" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q409" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R409" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S409" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T409" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U409" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V409" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W409" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X409" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y409" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z409" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA409" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB409" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC409" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD409" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="410" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A410" s="4">
+        <v>45571.984171504635</v>
+      </c>
+      <c r="B410" s="5" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C410" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D410" s="5">
+        <v>20223010</v>
+      </c>
+      <c r="E410" s="5" t="s">
+        <v>1013</v>
+      </c>
+      <c r="F410" s="5">
+        <v>3</v>
+      </c>
+      <c r="G410" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H410" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I410" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J410" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K410" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L410" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M410" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N410" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O410" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P410" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q410" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R410" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S410" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T410" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U410" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V410" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W410" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X410" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y410" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z410" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA410" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB410" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC410" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD410" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="411" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A411" s="7">
+        <v>45571.989378796294</v>
+      </c>
+      <c r="B411" s="8" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C411" s="8" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D411" s="8">
+        <v>20233846</v>
+      </c>
+      <c r="E411" s="8" t="s">
+        <v>1016</v>
+      </c>
+      <c r="F411" s="8">
+        <v>3</v>
+      </c>
+      <c r="G411" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H411" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I411" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J411" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K411" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L411" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M411" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N411" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O411" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P411" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q411" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R411" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S411" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T411" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U411" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V411" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W411" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X411" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y411" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z411" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA411" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB411" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC411" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD411" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="412" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A412" s="4">
+        <v>45571.99716107639</v>
+      </c>
+      <c r="B412" s="5" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C412" s="5" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D412" s="5">
+        <v>20203352</v>
+      </c>
+      <c r="E412" s="5" t="s">
+        <v>1019</v>
+      </c>
+      <c r="F412" s="5">
+        <v>3</v>
+      </c>
+      <c r="G412" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H412" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I412" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J412" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="K412" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L412" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M412" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N412" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O412" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P412" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q412" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R412" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S412" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T412" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="U412" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V412" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W412" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X412" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y412" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z412" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA412" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB412" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC412" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD412" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="413" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A413" s="7">
+        <v>45571.997394479171</v>
+      </c>
+      <c r="B413" s="8" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C413" s="8" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D413" s="8">
+        <v>20233930</v>
+      </c>
+      <c r="E413" s="8" t="s">
+        <v>1022</v>
+      </c>
+      <c r="F413" s="8">
+        <v>3</v>
+      </c>
+      <c r="G413" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H413" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I413" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J413" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K413" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L413" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M413" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N413" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O413" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P413" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q413" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R413" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S413" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T413" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U413" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V413" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="W413" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X413" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y413" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z413" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA413" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB413" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC413" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD413" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="414" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A414" s="4">
+        <v>45572.004169259264</v>
+      </c>
+      <c r="B414" s="5" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C414" s="5" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D414" s="5">
+        <v>20245218</v>
+      </c>
+      <c r="E414" s="5" t="s">
+        <v>1025</v>
+      </c>
+      <c r="F414" s="5">
+        <v>3</v>
+      </c>
+      <c r="G414" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H414" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I414" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J414" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K414" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="L414" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M414" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N414" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O414" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P414" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q414" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R414" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S414" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T414" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U414" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V414" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W414" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X414" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y414" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z414" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA414" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB414" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC414" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD414" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="415" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A415" s="13">
+        <v>45572.011804652779</v>
+      </c>
+      <c r="B415" s="14" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C415" s="14" t="s">
+        <v>497</v>
+      </c>
+      <c r="D415" s="14">
+        <v>20246902</v>
+      </c>
+      <c r="E415" s="14" t="s">
+        <v>1027</v>
+      </c>
+      <c r="F415" s="14">
+        <v>4</v>
+      </c>
+      <c r="G415" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H415" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="I415" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="J415" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="K415" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="L415" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="M415" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N415" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="O415" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="P415" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q415" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="R415" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="S415" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="T415" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="U415" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="V415" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="W415" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="X415" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="Y415" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z415" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA415" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB415" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="AC415" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD415" s="15" t="s">
+        <v>214</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>